<commit_message>
update Unit Test Results
</commit_message>
<xml_diff>
--- a/Unit Test Results/DistrictDao.xlsx
+++ b/Unit Test Results/DistrictDao.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Delete" sheetId="1" r:id="rId1"/>
@@ -363,9 +363,6 @@
     <t>6, null, 1</t>
   </si>
   <si>
-    <t>6, Một cái tên xa lạ, null</t>
-  </si>
-  <si>
     <t>null id, Hoàng Cầu, 1</t>
   </si>
   <si>
@@ -378,7 +375,10 @@
     <t>1234, Hai Bà Trưng, 1</t>
   </si>
   <si>
-    <t>6, Hai Bà Trưng, null</t>
+    <t>6, Hai Bà Trưng</t>
+  </si>
+  <si>
+    <t>6, Một cái tên xa lạ</t>
   </si>
 </sst>
 </file>
@@ -1154,6 +1154,102 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment textRotation="255"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1171,102 +1267,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1578,7 +1578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -2039,51 +2039,51 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:26">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="93"/>
-      <c r="F2" s="94" t="s">
+      <c r="B2" s="64"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="66"/>
+      <c r="F2" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="96"/>
-      <c r="S2" s="96"/>
-      <c r="T2" s="97"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="69"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="69"/>
+      <c r="T2" s="70"/>
     </row>
     <row r="3" spans="1:26">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="98" t="s">
+      <c r="B3" s="72"/>
+      <c r="C3" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="99"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="82" t="s">
+      <c r="D3" s="74"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="88"/>
-      <c r="N3" s="88"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
@@ -2092,112 +2092,112 @@
       <c r="T3" s="6"/>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="79"/>
+      <c r="B4" s="72"/>
       <c r="C4" s="80"/>
       <c r="D4" s="81"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="82" t="s">
+      <c r="F4" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="84"/>
-      <c r="M4" s="85"/>
-      <c r="N4" s="85"/>
-      <c r="O4" s="85"/>
-      <c r="P4" s="85"/>
-      <c r="Q4" s="85"/>
-      <c r="R4" s="85"/>
-      <c r="S4" s="85"/>
-      <c r="T4" s="86"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="83"/>
+      <c r="P4" s="83"/>
+      <c r="Q4" s="83"/>
+      <c r="R4" s="83"/>
+      <c r="S4" s="83"/>
+      <c r="T4" s="84"/>
       <c r="V4" s="8"/>
     </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="87" t="s">
+      <c r="B5" s="72"/>
+      <c r="C5" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="88"/>
-      <c r="K5" s="88"/>
-      <c r="L5" s="88"/>
-      <c r="M5" s="88"/>
-      <c r="N5" s="88"/>
-      <c r="O5" s="88"/>
-      <c r="P5" s="88"/>
-      <c r="Q5" s="88"/>
-      <c r="R5" s="88"/>
-      <c r="S5" s="88"/>
-      <c r="T5" s="89"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="79"/>
+      <c r="Q5" s="79"/>
+      <c r="R5" s="79"/>
+      <c r="S5" s="79"/>
+      <c r="T5" s="85"/>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="69" t="s">
+      <c r="B6" s="100"/>
+      <c r="C6" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="70"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="69" t="s">
+      <c r="D6" s="87"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="69" t="s">
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="88"/>
+      <c r="L6" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="70"/>
-      <c r="N6" s="71"/>
-      <c r="O6" s="69" t="s">
+      <c r="M6" s="87"/>
+      <c r="N6" s="88"/>
+      <c r="O6" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="70"/>
-      <c r="Q6" s="70"/>
-      <c r="R6" s="70"/>
-      <c r="S6" s="70"/>
-      <c r="T6" s="72"/>
+      <c r="P6" s="87"/>
+      <c r="Q6" s="87"/>
+      <c r="R6" s="87"/>
+      <c r="S6" s="87"/>
+      <c r="T6" s="89"/>
       <c r="V6" s="8"/>
     </row>
     <row r="7" spans="1:26" ht="11.25" thickBot="1">
-      <c r="A7" s="73">
+      <c r="A7" s="90">
         <f>COUNTIF(F23:HQ23,"P")</f>
         <v>2</v>
       </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="75">
+      <c r="B7" s="91"/>
+      <c r="C7" s="92">
         <f>COUNTIF(F23:HQ23,"F")</f>
         <v>0</v>
       </c>
-      <c r="D7" s="76"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="75">
+      <c r="D7" s="93"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="92">
         <f>SUM(O7,-A7,-C7)</f>
         <v>19</v>
       </c>
-      <c r="G7" s="76"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="76"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="74"/>
+      <c r="G7" s="93"/>
+      <c r="H7" s="93"/>
+      <c r="I7" s="93"/>
+      <c r="J7" s="93"/>
+      <c r="K7" s="91"/>
       <c r="L7" s="9">
         <f>COUNTIF(E22:HQ22,"N")</f>
         <v>0</v>
@@ -2210,15 +2210,15 @@
         <f>COUNTIF(E22:HQ22,"B")</f>
         <v>0</v>
       </c>
-      <c r="O7" s="75">
+      <c r="O7" s="92">
         <f>COUNTA(E9:HT9)</f>
         <v>21</v>
       </c>
-      <c r="P7" s="76"/>
-      <c r="Q7" s="76"/>
-      <c r="R7" s="76"/>
-      <c r="S7" s="76"/>
-      <c r="T7" s="77"/>
+      <c r="P7" s="93"/>
+      <c r="Q7" s="93"/>
+      <c r="R7" s="93"/>
+      <c r="S7" s="93"/>
+      <c r="T7" s="94"/>
       <c r="U7" s="10"/>
     </row>
     <row r="8" spans="1:26" ht="11.25" thickBot="1"/>
@@ -2660,11 +2660,11 @@
       <c r="A22" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="63" t="s">
+      <c r="B22" s="95" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="95"/>
       <c r="E22" s="49"/>
       <c r="F22" s="50"/>
       <c r="G22" s="50"/>
@@ -2690,11 +2690,11 @@
     </row>
     <row r="23" spans="1:26" ht="11.25">
       <c r="A23" s="52"/>
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="96" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="96"/>
       <c r="E23" s="53"/>
       <c r="F23" s="54" t="s">
         <v>46</v>
@@ -2724,11 +2724,11 @@
     </row>
     <row r="24" spans="1:26">
       <c r="A24" s="52"/>
-      <c r="B24" s="65" t="s">
+      <c r="B24" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
+      <c r="C24" s="97"/>
+      <c r="D24" s="97"/>
       <c r="E24" s="56"/>
       <c r="F24" s="57"/>
       <c r="G24" s="57"/>
@@ -2754,11 +2754,11 @@
     </row>
     <row r="25" spans="1:26" ht="11.25" thickBot="1">
       <c r="A25" s="59"/>
-      <c r="B25" s="66" t="s">
+      <c r="B25" s="98" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="66"/>
-      <c r="D25" s="66"/>
+      <c r="C25" s="98"/>
+      <c r="D25" s="98"/>
       <c r="E25" s="60"/>
       <c r="F25" s="61"/>
       <c r="G25" s="61"/>
@@ -2790,6 +2790,25 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:K6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="O6:T6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:K7"/>
+    <mergeCell ref="O7:T7"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="L4:T4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:T5"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:K2"/>
@@ -2798,25 +2817,6 @@
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="F3:K3"/>
     <mergeCell ref="L3:N3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:K4"/>
-    <mergeCell ref="L4:T4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:T5"/>
-    <mergeCell ref="F6:K6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="O6:T6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:K7"/>
-    <mergeCell ref="O7:T7"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F10:T21 JB10:JP21 SX10:TL21 ACT10:ADH21 AMP10:AND21 AWL10:AWZ21 BGH10:BGV21 BQD10:BQR21 BZZ10:CAN21 CJV10:CKJ21 CTR10:CUF21 DDN10:DEB21 DNJ10:DNX21 DXF10:DXT21 EHB10:EHP21 EQX10:ERL21 FAT10:FBH21 FKP10:FLD21 FUL10:FUZ21 GEH10:GEV21 GOD10:GOR21 GXZ10:GYN21 HHV10:HIJ21 HRR10:HSF21 IBN10:ICB21 ILJ10:ILX21 IVF10:IVT21 JFB10:JFP21 JOX10:JPL21 JYT10:JZH21 KIP10:KJD21 KSL10:KSZ21 LCH10:LCV21 LMD10:LMR21 LVZ10:LWN21 MFV10:MGJ21 MPR10:MQF21 MZN10:NAB21 NJJ10:NJX21 NTF10:NTT21 ODB10:ODP21 OMX10:ONL21 OWT10:OXH21 PGP10:PHD21 PQL10:PQZ21 QAH10:QAV21 QKD10:QKR21 QTZ10:QUN21 RDV10:REJ21 RNR10:ROF21 RXN10:RYB21 SHJ10:SHX21 SRF10:SRT21 TBB10:TBP21 TKX10:TLL21 TUT10:TVH21 UEP10:UFD21 UOL10:UOZ21 UYH10:UYV21 VID10:VIR21 VRZ10:VSN21 WBV10:WCJ21 WLR10:WMF21 WVN10:WWB21 F65546:T65557 JB65546:JP65557 SX65546:TL65557 ACT65546:ADH65557 AMP65546:AND65557 AWL65546:AWZ65557 BGH65546:BGV65557 BQD65546:BQR65557 BZZ65546:CAN65557 CJV65546:CKJ65557 CTR65546:CUF65557 DDN65546:DEB65557 DNJ65546:DNX65557 DXF65546:DXT65557 EHB65546:EHP65557 EQX65546:ERL65557 FAT65546:FBH65557 FKP65546:FLD65557 FUL65546:FUZ65557 GEH65546:GEV65557 GOD65546:GOR65557 GXZ65546:GYN65557 HHV65546:HIJ65557 HRR65546:HSF65557 IBN65546:ICB65557 ILJ65546:ILX65557 IVF65546:IVT65557 JFB65546:JFP65557 JOX65546:JPL65557 JYT65546:JZH65557 KIP65546:KJD65557 KSL65546:KSZ65557 LCH65546:LCV65557 LMD65546:LMR65557 LVZ65546:LWN65557 MFV65546:MGJ65557 MPR65546:MQF65557 MZN65546:NAB65557 NJJ65546:NJX65557 NTF65546:NTT65557 ODB65546:ODP65557 OMX65546:ONL65557 OWT65546:OXH65557 PGP65546:PHD65557 PQL65546:PQZ65557 QAH65546:QAV65557 QKD65546:QKR65557 QTZ65546:QUN65557 RDV65546:REJ65557 RNR65546:ROF65557 RXN65546:RYB65557 SHJ65546:SHX65557 SRF65546:SRT65557 TBB65546:TBP65557 TKX65546:TLL65557 TUT65546:TVH65557 UEP65546:UFD65557 UOL65546:UOZ65557 UYH65546:UYV65557 VID65546:VIR65557 VRZ65546:VSN65557 WBV65546:WCJ65557 WLR65546:WMF65557 WVN65546:WWB65557 F131082:T131093 JB131082:JP131093 SX131082:TL131093 ACT131082:ADH131093 AMP131082:AND131093 AWL131082:AWZ131093 BGH131082:BGV131093 BQD131082:BQR131093 BZZ131082:CAN131093 CJV131082:CKJ131093 CTR131082:CUF131093 DDN131082:DEB131093 DNJ131082:DNX131093 DXF131082:DXT131093 EHB131082:EHP131093 EQX131082:ERL131093 FAT131082:FBH131093 FKP131082:FLD131093 FUL131082:FUZ131093 GEH131082:GEV131093 GOD131082:GOR131093 GXZ131082:GYN131093 HHV131082:HIJ131093 HRR131082:HSF131093 IBN131082:ICB131093 ILJ131082:ILX131093 IVF131082:IVT131093 JFB131082:JFP131093 JOX131082:JPL131093 JYT131082:JZH131093 KIP131082:KJD131093 KSL131082:KSZ131093 LCH131082:LCV131093 LMD131082:LMR131093 LVZ131082:LWN131093 MFV131082:MGJ131093 MPR131082:MQF131093 MZN131082:NAB131093 NJJ131082:NJX131093 NTF131082:NTT131093 ODB131082:ODP131093 OMX131082:ONL131093 OWT131082:OXH131093 PGP131082:PHD131093 PQL131082:PQZ131093 QAH131082:QAV131093 QKD131082:QKR131093 QTZ131082:QUN131093 RDV131082:REJ131093 RNR131082:ROF131093 RXN131082:RYB131093 SHJ131082:SHX131093 SRF131082:SRT131093 TBB131082:TBP131093 TKX131082:TLL131093 TUT131082:TVH131093 UEP131082:UFD131093 UOL131082:UOZ131093 UYH131082:UYV131093 VID131082:VIR131093 VRZ131082:VSN131093 WBV131082:WCJ131093 WLR131082:WMF131093 WVN131082:WWB131093 F196618:T196629 JB196618:JP196629 SX196618:TL196629 ACT196618:ADH196629 AMP196618:AND196629 AWL196618:AWZ196629 BGH196618:BGV196629 BQD196618:BQR196629 BZZ196618:CAN196629 CJV196618:CKJ196629 CTR196618:CUF196629 DDN196618:DEB196629 DNJ196618:DNX196629 DXF196618:DXT196629 EHB196618:EHP196629 EQX196618:ERL196629 FAT196618:FBH196629 FKP196618:FLD196629 FUL196618:FUZ196629 GEH196618:GEV196629 GOD196618:GOR196629 GXZ196618:GYN196629 HHV196618:HIJ196629 HRR196618:HSF196629 IBN196618:ICB196629 ILJ196618:ILX196629 IVF196618:IVT196629 JFB196618:JFP196629 JOX196618:JPL196629 JYT196618:JZH196629 KIP196618:KJD196629 KSL196618:KSZ196629 LCH196618:LCV196629 LMD196618:LMR196629 LVZ196618:LWN196629 MFV196618:MGJ196629 MPR196618:MQF196629 MZN196618:NAB196629 NJJ196618:NJX196629 NTF196618:NTT196629 ODB196618:ODP196629 OMX196618:ONL196629 OWT196618:OXH196629 PGP196618:PHD196629 PQL196618:PQZ196629 QAH196618:QAV196629 QKD196618:QKR196629 QTZ196618:QUN196629 RDV196618:REJ196629 RNR196618:ROF196629 RXN196618:RYB196629 SHJ196618:SHX196629 SRF196618:SRT196629 TBB196618:TBP196629 TKX196618:TLL196629 TUT196618:TVH196629 UEP196618:UFD196629 UOL196618:UOZ196629 UYH196618:UYV196629 VID196618:VIR196629 VRZ196618:VSN196629 WBV196618:WCJ196629 WLR196618:WMF196629 WVN196618:WWB196629 F262154:T262165 JB262154:JP262165 SX262154:TL262165 ACT262154:ADH262165 AMP262154:AND262165 AWL262154:AWZ262165 BGH262154:BGV262165 BQD262154:BQR262165 BZZ262154:CAN262165 CJV262154:CKJ262165 CTR262154:CUF262165 DDN262154:DEB262165 DNJ262154:DNX262165 DXF262154:DXT262165 EHB262154:EHP262165 EQX262154:ERL262165 FAT262154:FBH262165 FKP262154:FLD262165 FUL262154:FUZ262165 GEH262154:GEV262165 GOD262154:GOR262165 GXZ262154:GYN262165 HHV262154:HIJ262165 HRR262154:HSF262165 IBN262154:ICB262165 ILJ262154:ILX262165 IVF262154:IVT262165 JFB262154:JFP262165 JOX262154:JPL262165 JYT262154:JZH262165 KIP262154:KJD262165 KSL262154:KSZ262165 LCH262154:LCV262165 LMD262154:LMR262165 LVZ262154:LWN262165 MFV262154:MGJ262165 MPR262154:MQF262165 MZN262154:NAB262165 NJJ262154:NJX262165 NTF262154:NTT262165 ODB262154:ODP262165 OMX262154:ONL262165 OWT262154:OXH262165 PGP262154:PHD262165 PQL262154:PQZ262165 QAH262154:QAV262165 QKD262154:QKR262165 QTZ262154:QUN262165 RDV262154:REJ262165 RNR262154:ROF262165 RXN262154:RYB262165 SHJ262154:SHX262165 SRF262154:SRT262165 TBB262154:TBP262165 TKX262154:TLL262165 TUT262154:TVH262165 UEP262154:UFD262165 UOL262154:UOZ262165 UYH262154:UYV262165 VID262154:VIR262165 VRZ262154:VSN262165 WBV262154:WCJ262165 WLR262154:WMF262165 WVN262154:WWB262165 F327690:T327701 JB327690:JP327701 SX327690:TL327701 ACT327690:ADH327701 AMP327690:AND327701 AWL327690:AWZ327701 BGH327690:BGV327701 BQD327690:BQR327701 BZZ327690:CAN327701 CJV327690:CKJ327701 CTR327690:CUF327701 DDN327690:DEB327701 DNJ327690:DNX327701 DXF327690:DXT327701 EHB327690:EHP327701 EQX327690:ERL327701 FAT327690:FBH327701 FKP327690:FLD327701 FUL327690:FUZ327701 GEH327690:GEV327701 GOD327690:GOR327701 GXZ327690:GYN327701 HHV327690:HIJ327701 HRR327690:HSF327701 IBN327690:ICB327701 ILJ327690:ILX327701 IVF327690:IVT327701 JFB327690:JFP327701 JOX327690:JPL327701 JYT327690:JZH327701 KIP327690:KJD327701 KSL327690:KSZ327701 LCH327690:LCV327701 LMD327690:LMR327701 LVZ327690:LWN327701 MFV327690:MGJ327701 MPR327690:MQF327701 MZN327690:NAB327701 NJJ327690:NJX327701 NTF327690:NTT327701 ODB327690:ODP327701 OMX327690:ONL327701 OWT327690:OXH327701 PGP327690:PHD327701 PQL327690:PQZ327701 QAH327690:QAV327701 QKD327690:QKR327701 QTZ327690:QUN327701 RDV327690:REJ327701 RNR327690:ROF327701 RXN327690:RYB327701 SHJ327690:SHX327701 SRF327690:SRT327701 TBB327690:TBP327701 TKX327690:TLL327701 TUT327690:TVH327701 UEP327690:UFD327701 UOL327690:UOZ327701 UYH327690:UYV327701 VID327690:VIR327701 VRZ327690:VSN327701 WBV327690:WCJ327701 WLR327690:WMF327701 WVN327690:WWB327701 F393226:T393237 JB393226:JP393237 SX393226:TL393237 ACT393226:ADH393237 AMP393226:AND393237 AWL393226:AWZ393237 BGH393226:BGV393237 BQD393226:BQR393237 BZZ393226:CAN393237 CJV393226:CKJ393237 CTR393226:CUF393237 DDN393226:DEB393237 DNJ393226:DNX393237 DXF393226:DXT393237 EHB393226:EHP393237 EQX393226:ERL393237 FAT393226:FBH393237 FKP393226:FLD393237 FUL393226:FUZ393237 GEH393226:GEV393237 GOD393226:GOR393237 GXZ393226:GYN393237 HHV393226:HIJ393237 HRR393226:HSF393237 IBN393226:ICB393237 ILJ393226:ILX393237 IVF393226:IVT393237 JFB393226:JFP393237 JOX393226:JPL393237 JYT393226:JZH393237 KIP393226:KJD393237 KSL393226:KSZ393237 LCH393226:LCV393237 LMD393226:LMR393237 LVZ393226:LWN393237 MFV393226:MGJ393237 MPR393226:MQF393237 MZN393226:NAB393237 NJJ393226:NJX393237 NTF393226:NTT393237 ODB393226:ODP393237 OMX393226:ONL393237 OWT393226:OXH393237 PGP393226:PHD393237 PQL393226:PQZ393237 QAH393226:QAV393237 QKD393226:QKR393237 QTZ393226:QUN393237 RDV393226:REJ393237 RNR393226:ROF393237 RXN393226:RYB393237 SHJ393226:SHX393237 SRF393226:SRT393237 TBB393226:TBP393237 TKX393226:TLL393237 TUT393226:TVH393237 UEP393226:UFD393237 UOL393226:UOZ393237 UYH393226:UYV393237 VID393226:VIR393237 VRZ393226:VSN393237 WBV393226:WCJ393237 WLR393226:WMF393237 WVN393226:WWB393237 F458762:T458773 JB458762:JP458773 SX458762:TL458773 ACT458762:ADH458773 AMP458762:AND458773 AWL458762:AWZ458773 BGH458762:BGV458773 BQD458762:BQR458773 BZZ458762:CAN458773 CJV458762:CKJ458773 CTR458762:CUF458773 DDN458762:DEB458773 DNJ458762:DNX458773 DXF458762:DXT458773 EHB458762:EHP458773 EQX458762:ERL458773 FAT458762:FBH458773 FKP458762:FLD458773 FUL458762:FUZ458773 GEH458762:GEV458773 GOD458762:GOR458773 GXZ458762:GYN458773 HHV458762:HIJ458773 HRR458762:HSF458773 IBN458762:ICB458773 ILJ458762:ILX458773 IVF458762:IVT458773 JFB458762:JFP458773 JOX458762:JPL458773 JYT458762:JZH458773 KIP458762:KJD458773 KSL458762:KSZ458773 LCH458762:LCV458773 LMD458762:LMR458773 LVZ458762:LWN458773 MFV458762:MGJ458773 MPR458762:MQF458773 MZN458762:NAB458773 NJJ458762:NJX458773 NTF458762:NTT458773 ODB458762:ODP458773 OMX458762:ONL458773 OWT458762:OXH458773 PGP458762:PHD458773 PQL458762:PQZ458773 QAH458762:QAV458773 QKD458762:QKR458773 QTZ458762:QUN458773 RDV458762:REJ458773 RNR458762:ROF458773 RXN458762:RYB458773 SHJ458762:SHX458773 SRF458762:SRT458773 TBB458762:TBP458773 TKX458762:TLL458773 TUT458762:TVH458773 UEP458762:UFD458773 UOL458762:UOZ458773 UYH458762:UYV458773 VID458762:VIR458773 VRZ458762:VSN458773 WBV458762:WCJ458773 WLR458762:WMF458773 WVN458762:WWB458773 F524298:T524309 JB524298:JP524309 SX524298:TL524309 ACT524298:ADH524309 AMP524298:AND524309 AWL524298:AWZ524309 BGH524298:BGV524309 BQD524298:BQR524309 BZZ524298:CAN524309 CJV524298:CKJ524309 CTR524298:CUF524309 DDN524298:DEB524309 DNJ524298:DNX524309 DXF524298:DXT524309 EHB524298:EHP524309 EQX524298:ERL524309 FAT524298:FBH524309 FKP524298:FLD524309 FUL524298:FUZ524309 GEH524298:GEV524309 GOD524298:GOR524309 GXZ524298:GYN524309 HHV524298:HIJ524309 HRR524298:HSF524309 IBN524298:ICB524309 ILJ524298:ILX524309 IVF524298:IVT524309 JFB524298:JFP524309 JOX524298:JPL524309 JYT524298:JZH524309 KIP524298:KJD524309 KSL524298:KSZ524309 LCH524298:LCV524309 LMD524298:LMR524309 LVZ524298:LWN524309 MFV524298:MGJ524309 MPR524298:MQF524309 MZN524298:NAB524309 NJJ524298:NJX524309 NTF524298:NTT524309 ODB524298:ODP524309 OMX524298:ONL524309 OWT524298:OXH524309 PGP524298:PHD524309 PQL524298:PQZ524309 QAH524298:QAV524309 QKD524298:QKR524309 QTZ524298:QUN524309 RDV524298:REJ524309 RNR524298:ROF524309 RXN524298:RYB524309 SHJ524298:SHX524309 SRF524298:SRT524309 TBB524298:TBP524309 TKX524298:TLL524309 TUT524298:TVH524309 UEP524298:UFD524309 UOL524298:UOZ524309 UYH524298:UYV524309 VID524298:VIR524309 VRZ524298:VSN524309 WBV524298:WCJ524309 WLR524298:WMF524309 WVN524298:WWB524309 F589834:T589845 JB589834:JP589845 SX589834:TL589845 ACT589834:ADH589845 AMP589834:AND589845 AWL589834:AWZ589845 BGH589834:BGV589845 BQD589834:BQR589845 BZZ589834:CAN589845 CJV589834:CKJ589845 CTR589834:CUF589845 DDN589834:DEB589845 DNJ589834:DNX589845 DXF589834:DXT589845 EHB589834:EHP589845 EQX589834:ERL589845 FAT589834:FBH589845 FKP589834:FLD589845 FUL589834:FUZ589845 GEH589834:GEV589845 GOD589834:GOR589845 GXZ589834:GYN589845 HHV589834:HIJ589845 HRR589834:HSF589845 IBN589834:ICB589845 ILJ589834:ILX589845 IVF589834:IVT589845 JFB589834:JFP589845 JOX589834:JPL589845 JYT589834:JZH589845 KIP589834:KJD589845 KSL589834:KSZ589845 LCH589834:LCV589845 LMD589834:LMR589845 LVZ589834:LWN589845 MFV589834:MGJ589845 MPR589834:MQF589845 MZN589834:NAB589845 NJJ589834:NJX589845 NTF589834:NTT589845 ODB589834:ODP589845 OMX589834:ONL589845 OWT589834:OXH589845 PGP589834:PHD589845 PQL589834:PQZ589845 QAH589834:QAV589845 QKD589834:QKR589845 QTZ589834:QUN589845 RDV589834:REJ589845 RNR589834:ROF589845 RXN589834:RYB589845 SHJ589834:SHX589845 SRF589834:SRT589845 TBB589834:TBP589845 TKX589834:TLL589845 TUT589834:TVH589845 UEP589834:UFD589845 UOL589834:UOZ589845 UYH589834:UYV589845 VID589834:VIR589845 VRZ589834:VSN589845 WBV589834:WCJ589845 WLR589834:WMF589845 WVN589834:WWB589845 F655370:T655381 JB655370:JP655381 SX655370:TL655381 ACT655370:ADH655381 AMP655370:AND655381 AWL655370:AWZ655381 BGH655370:BGV655381 BQD655370:BQR655381 BZZ655370:CAN655381 CJV655370:CKJ655381 CTR655370:CUF655381 DDN655370:DEB655381 DNJ655370:DNX655381 DXF655370:DXT655381 EHB655370:EHP655381 EQX655370:ERL655381 FAT655370:FBH655381 FKP655370:FLD655381 FUL655370:FUZ655381 GEH655370:GEV655381 GOD655370:GOR655381 GXZ655370:GYN655381 HHV655370:HIJ655381 HRR655370:HSF655381 IBN655370:ICB655381 ILJ655370:ILX655381 IVF655370:IVT655381 JFB655370:JFP655381 JOX655370:JPL655381 JYT655370:JZH655381 KIP655370:KJD655381 KSL655370:KSZ655381 LCH655370:LCV655381 LMD655370:LMR655381 LVZ655370:LWN655381 MFV655370:MGJ655381 MPR655370:MQF655381 MZN655370:NAB655381 NJJ655370:NJX655381 NTF655370:NTT655381 ODB655370:ODP655381 OMX655370:ONL655381 OWT655370:OXH655381 PGP655370:PHD655381 PQL655370:PQZ655381 QAH655370:QAV655381 QKD655370:QKR655381 QTZ655370:QUN655381 RDV655370:REJ655381 RNR655370:ROF655381 RXN655370:RYB655381 SHJ655370:SHX655381 SRF655370:SRT655381 TBB655370:TBP655381 TKX655370:TLL655381 TUT655370:TVH655381 UEP655370:UFD655381 UOL655370:UOZ655381 UYH655370:UYV655381 VID655370:VIR655381 VRZ655370:VSN655381 WBV655370:WCJ655381 WLR655370:WMF655381 WVN655370:WWB655381 F720906:T720917 JB720906:JP720917 SX720906:TL720917 ACT720906:ADH720917 AMP720906:AND720917 AWL720906:AWZ720917 BGH720906:BGV720917 BQD720906:BQR720917 BZZ720906:CAN720917 CJV720906:CKJ720917 CTR720906:CUF720917 DDN720906:DEB720917 DNJ720906:DNX720917 DXF720906:DXT720917 EHB720906:EHP720917 EQX720906:ERL720917 FAT720906:FBH720917 FKP720906:FLD720917 FUL720906:FUZ720917 GEH720906:GEV720917 GOD720906:GOR720917 GXZ720906:GYN720917 HHV720906:HIJ720917 HRR720906:HSF720917 IBN720906:ICB720917 ILJ720906:ILX720917 IVF720906:IVT720917 JFB720906:JFP720917 JOX720906:JPL720917 JYT720906:JZH720917 KIP720906:KJD720917 KSL720906:KSZ720917 LCH720906:LCV720917 LMD720906:LMR720917 LVZ720906:LWN720917 MFV720906:MGJ720917 MPR720906:MQF720917 MZN720906:NAB720917 NJJ720906:NJX720917 NTF720906:NTT720917 ODB720906:ODP720917 OMX720906:ONL720917 OWT720906:OXH720917 PGP720906:PHD720917 PQL720906:PQZ720917 QAH720906:QAV720917 QKD720906:QKR720917 QTZ720906:QUN720917 RDV720906:REJ720917 RNR720906:ROF720917 RXN720906:RYB720917 SHJ720906:SHX720917 SRF720906:SRT720917 TBB720906:TBP720917 TKX720906:TLL720917 TUT720906:TVH720917 UEP720906:UFD720917 UOL720906:UOZ720917 UYH720906:UYV720917 VID720906:VIR720917 VRZ720906:VSN720917 WBV720906:WCJ720917 WLR720906:WMF720917 WVN720906:WWB720917 F786442:T786453 JB786442:JP786453 SX786442:TL786453 ACT786442:ADH786453 AMP786442:AND786453 AWL786442:AWZ786453 BGH786442:BGV786453 BQD786442:BQR786453 BZZ786442:CAN786453 CJV786442:CKJ786453 CTR786442:CUF786453 DDN786442:DEB786453 DNJ786442:DNX786453 DXF786442:DXT786453 EHB786442:EHP786453 EQX786442:ERL786453 FAT786442:FBH786453 FKP786442:FLD786453 FUL786442:FUZ786453 GEH786442:GEV786453 GOD786442:GOR786453 GXZ786442:GYN786453 HHV786442:HIJ786453 HRR786442:HSF786453 IBN786442:ICB786453 ILJ786442:ILX786453 IVF786442:IVT786453 JFB786442:JFP786453 JOX786442:JPL786453 JYT786442:JZH786453 KIP786442:KJD786453 KSL786442:KSZ786453 LCH786442:LCV786453 LMD786442:LMR786453 LVZ786442:LWN786453 MFV786442:MGJ786453 MPR786442:MQF786453 MZN786442:NAB786453 NJJ786442:NJX786453 NTF786442:NTT786453 ODB786442:ODP786453 OMX786442:ONL786453 OWT786442:OXH786453 PGP786442:PHD786453 PQL786442:PQZ786453 QAH786442:QAV786453 QKD786442:QKR786453 QTZ786442:QUN786453 RDV786442:REJ786453 RNR786442:ROF786453 RXN786442:RYB786453 SHJ786442:SHX786453 SRF786442:SRT786453 TBB786442:TBP786453 TKX786442:TLL786453 TUT786442:TVH786453 UEP786442:UFD786453 UOL786442:UOZ786453 UYH786442:UYV786453 VID786442:VIR786453 VRZ786442:VSN786453 WBV786442:WCJ786453 WLR786442:WMF786453 WVN786442:WWB786453 F851978:T851989 JB851978:JP851989 SX851978:TL851989 ACT851978:ADH851989 AMP851978:AND851989 AWL851978:AWZ851989 BGH851978:BGV851989 BQD851978:BQR851989 BZZ851978:CAN851989 CJV851978:CKJ851989 CTR851978:CUF851989 DDN851978:DEB851989 DNJ851978:DNX851989 DXF851978:DXT851989 EHB851978:EHP851989 EQX851978:ERL851989 FAT851978:FBH851989 FKP851978:FLD851989 FUL851978:FUZ851989 GEH851978:GEV851989 GOD851978:GOR851989 GXZ851978:GYN851989 HHV851978:HIJ851989 HRR851978:HSF851989 IBN851978:ICB851989 ILJ851978:ILX851989 IVF851978:IVT851989 JFB851978:JFP851989 JOX851978:JPL851989 JYT851978:JZH851989 KIP851978:KJD851989 KSL851978:KSZ851989 LCH851978:LCV851989 LMD851978:LMR851989 LVZ851978:LWN851989 MFV851978:MGJ851989 MPR851978:MQF851989 MZN851978:NAB851989 NJJ851978:NJX851989 NTF851978:NTT851989 ODB851978:ODP851989 OMX851978:ONL851989 OWT851978:OXH851989 PGP851978:PHD851989 PQL851978:PQZ851989 QAH851978:QAV851989 QKD851978:QKR851989 QTZ851978:QUN851989 RDV851978:REJ851989 RNR851978:ROF851989 RXN851978:RYB851989 SHJ851978:SHX851989 SRF851978:SRT851989 TBB851978:TBP851989 TKX851978:TLL851989 TUT851978:TVH851989 UEP851978:UFD851989 UOL851978:UOZ851989 UYH851978:UYV851989 VID851978:VIR851989 VRZ851978:VSN851989 WBV851978:WCJ851989 WLR851978:WMF851989 WVN851978:WWB851989 F917514:T917525 JB917514:JP917525 SX917514:TL917525 ACT917514:ADH917525 AMP917514:AND917525 AWL917514:AWZ917525 BGH917514:BGV917525 BQD917514:BQR917525 BZZ917514:CAN917525 CJV917514:CKJ917525 CTR917514:CUF917525 DDN917514:DEB917525 DNJ917514:DNX917525 DXF917514:DXT917525 EHB917514:EHP917525 EQX917514:ERL917525 FAT917514:FBH917525 FKP917514:FLD917525 FUL917514:FUZ917525 GEH917514:GEV917525 GOD917514:GOR917525 GXZ917514:GYN917525 HHV917514:HIJ917525 HRR917514:HSF917525 IBN917514:ICB917525 ILJ917514:ILX917525 IVF917514:IVT917525 JFB917514:JFP917525 JOX917514:JPL917525 JYT917514:JZH917525 KIP917514:KJD917525 KSL917514:KSZ917525 LCH917514:LCV917525 LMD917514:LMR917525 LVZ917514:LWN917525 MFV917514:MGJ917525 MPR917514:MQF917525 MZN917514:NAB917525 NJJ917514:NJX917525 NTF917514:NTT917525 ODB917514:ODP917525 OMX917514:ONL917525 OWT917514:OXH917525 PGP917514:PHD917525 PQL917514:PQZ917525 QAH917514:QAV917525 QKD917514:QKR917525 QTZ917514:QUN917525 RDV917514:REJ917525 RNR917514:ROF917525 RXN917514:RYB917525 SHJ917514:SHX917525 SRF917514:SRT917525 TBB917514:TBP917525 TKX917514:TLL917525 TUT917514:TVH917525 UEP917514:UFD917525 UOL917514:UOZ917525 UYH917514:UYV917525 VID917514:VIR917525 VRZ917514:VSN917525 WBV917514:WCJ917525 WLR917514:WMF917525 WVN917514:WWB917525 F983050:T983061 JB983050:JP983061 SX983050:TL983061 ACT983050:ADH983061 AMP983050:AND983061 AWL983050:AWZ983061 BGH983050:BGV983061 BQD983050:BQR983061 BZZ983050:CAN983061 CJV983050:CKJ983061 CTR983050:CUF983061 DDN983050:DEB983061 DNJ983050:DNX983061 DXF983050:DXT983061 EHB983050:EHP983061 EQX983050:ERL983061 FAT983050:FBH983061 FKP983050:FLD983061 FUL983050:FUZ983061 GEH983050:GEV983061 GOD983050:GOR983061 GXZ983050:GYN983061 HHV983050:HIJ983061 HRR983050:HSF983061 IBN983050:ICB983061 ILJ983050:ILX983061 IVF983050:IVT983061 JFB983050:JFP983061 JOX983050:JPL983061 JYT983050:JZH983061 KIP983050:KJD983061 KSL983050:KSZ983061 LCH983050:LCV983061 LMD983050:LMR983061 LVZ983050:LWN983061 MFV983050:MGJ983061 MPR983050:MQF983061 MZN983050:NAB983061 NJJ983050:NJX983061 NTF983050:NTT983061 ODB983050:ODP983061 OMX983050:ONL983061 OWT983050:OXH983061 PGP983050:PHD983061 PQL983050:PQZ983061 QAH983050:QAV983061 QKD983050:QKR983061 QTZ983050:QUN983061 RDV983050:REJ983061 RNR983050:ROF983061 RXN983050:RYB983061 SHJ983050:SHX983061 SRF983050:SRT983061 TBB983050:TBP983061 TKX983050:TLL983061 TUT983050:TVH983061 UEP983050:UFD983061 UOL983050:UOZ983061 UYH983050:UYV983061 VID983050:VIR983061 VRZ983050:VSN983061 WBV983050:WCJ983061 WLR983050:WMF983061 WVN983050:WWB983061">
@@ -3302,51 +3302,51 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:26">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="93"/>
-      <c r="F2" s="94" t="s">
+      <c r="B2" s="64"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="66"/>
+      <c r="F2" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="96"/>
-      <c r="S2" s="96"/>
-      <c r="T2" s="97"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="69"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="69"/>
+      <c r="T2" s="70"/>
     </row>
     <row r="3" spans="1:26">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="98" t="s">
+      <c r="B3" s="72"/>
+      <c r="C3" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="99"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="82" t="s">
+      <c r="D3" s="74"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="88"/>
-      <c r="N3" s="88"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
@@ -3355,112 +3355,112 @@
       <c r="T3" s="6"/>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="79"/>
+      <c r="B4" s="72"/>
       <c r="C4" s="80"/>
       <c r="D4" s="81"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="82" t="s">
+      <c r="F4" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="84"/>
-      <c r="M4" s="85"/>
-      <c r="N4" s="85"/>
-      <c r="O4" s="85"/>
-      <c r="P4" s="85"/>
-      <c r="Q4" s="85"/>
-      <c r="R4" s="85"/>
-      <c r="S4" s="85"/>
-      <c r="T4" s="86"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="83"/>
+      <c r="P4" s="83"/>
+      <c r="Q4" s="83"/>
+      <c r="R4" s="83"/>
+      <c r="S4" s="83"/>
+      <c r="T4" s="84"/>
       <c r="V4" s="8"/>
     </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="87" t="s">
+      <c r="B5" s="72"/>
+      <c r="C5" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="88"/>
-      <c r="K5" s="88"/>
-      <c r="L5" s="88"/>
-      <c r="M5" s="88"/>
-      <c r="N5" s="88"/>
-      <c r="O5" s="88"/>
-      <c r="P5" s="88"/>
-      <c r="Q5" s="88"/>
-      <c r="R5" s="88"/>
-      <c r="S5" s="88"/>
-      <c r="T5" s="89"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="79"/>
+      <c r="Q5" s="79"/>
+      <c r="R5" s="79"/>
+      <c r="S5" s="79"/>
+      <c r="T5" s="85"/>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="69" t="s">
+      <c r="B6" s="100"/>
+      <c r="C6" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="70"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="69" t="s">
+      <c r="D6" s="87"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="69" t="s">
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="88"/>
+      <c r="L6" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="70"/>
-      <c r="N6" s="71"/>
-      <c r="O6" s="69" t="s">
+      <c r="M6" s="87"/>
+      <c r="N6" s="88"/>
+      <c r="O6" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="70"/>
-      <c r="Q6" s="70"/>
-      <c r="R6" s="70"/>
-      <c r="S6" s="70"/>
-      <c r="T6" s="72"/>
+      <c r="P6" s="87"/>
+      <c r="Q6" s="87"/>
+      <c r="R6" s="87"/>
+      <c r="S6" s="87"/>
+      <c r="T6" s="89"/>
       <c r="V6" s="8"/>
     </row>
     <row r="7" spans="1:26" ht="11.25" thickBot="1">
-      <c r="A7" s="73">
+      <c r="A7" s="90">
         <f>COUNTIF(F23:HQ23,"P")</f>
         <v>1</v>
       </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="75">
+      <c r="B7" s="91"/>
+      <c r="C7" s="92">
         <f>COUNTIF(F23:HQ23,"F")</f>
         <v>0</v>
       </c>
-      <c r="D7" s="76"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="75">
+      <c r="D7" s="93"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="92">
         <f>SUM(O7,-A7,-C7)</f>
         <v>20</v>
       </c>
-      <c r="G7" s="76"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="76"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="74"/>
+      <c r="G7" s="93"/>
+      <c r="H7" s="93"/>
+      <c r="I7" s="93"/>
+      <c r="J7" s="93"/>
+      <c r="K7" s="91"/>
       <c r="L7" s="9">
         <f>COUNTIF(E22:HQ22,"N")</f>
         <v>0</v>
@@ -3473,15 +3473,15 @@
         <f>COUNTIF(E22:HQ22,"B")</f>
         <v>0</v>
       </c>
-      <c r="O7" s="75">
+      <c r="O7" s="92">
         <f>COUNTA(E9:HT9)</f>
         <v>21</v>
       </c>
-      <c r="P7" s="76"/>
-      <c r="Q7" s="76"/>
-      <c r="R7" s="76"/>
-      <c r="S7" s="76"/>
-      <c r="T7" s="77"/>
+      <c r="P7" s="93"/>
+      <c r="Q7" s="93"/>
+      <c r="R7" s="93"/>
+      <c r="S7" s="93"/>
+      <c r="T7" s="94"/>
       <c r="U7" s="10"/>
     </row>
     <row r="8" spans="1:26" ht="11.25" thickBot="1"/>
@@ -3915,11 +3915,11 @@
       <c r="A22" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="63" t="s">
+      <c r="B22" s="95" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="95"/>
       <c r="E22" s="49"/>
       <c r="F22" s="50"/>
       <c r="G22" s="50"/>
@@ -3945,11 +3945,11 @@
     </row>
     <row r="23" spans="1:26" ht="11.25">
       <c r="A23" s="52"/>
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="96" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="96"/>
       <c r="E23" s="53"/>
       <c r="F23" s="54" t="s">
         <v>46</v>
@@ -3977,11 +3977,11 @@
     </row>
     <row r="24" spans="1:26">
       <c r="A24" s="52"/>
-      <c r="B24" s="65" t="s">
+      <c r="B24" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
+      <c r="C24" s="97"/>
+      <c r="D24" s="97"/>
       <c r="E24" s="56"/>
       <c r="F24" s="57"/>
       <c r="G24" s="57"/>
@@ -4007,11 +4007,11 @@
     </row>
     <row r="25" spans="1:26" ht="11.25" thickBot="1">
       <c r="A25" s="59"/>
-      <c r="B25" s="66" t="s">
+      <c r="B25" s="98" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="66"/>
-      <c r="D25" s="66"/>
+      <c r="C25" s="98"/>
+      <c r="D25" s="98"/>
       <c r="E25" s="60"/>
       <c r="F25" s="61"/>
       <c r="G25" s="61"/>
@@ -4043,6 +4043,25 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:K6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="O6:T6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:K7"/>
+    <mergeCell ref="O7:T7"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="L4:T4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:T5"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:K2"/>
@@ -4051,25 +4070,6 @@
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="F3:K3"/>
     <mergeCell ref="L3:N3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:K4"/>
-    <mergeCell ref="L4:T4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:T5"/>
-    <mergeCell ref="F6:K6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="O6:T6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:K7"/>
-    <mergeCell ref="O7:T7"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F10:T21 JB10:JP21 SX10:TL21 ACT10:ADH21 AMP10:AND21 AWL10:AWZ21 BGH10:BGV21 BQD10:BQR21 BZZ10:CAN21 CJV10:CKJ21 CTR10:CUF21 DDN10:DEB21 DNJ10:DNX21 DXF10:DXT21 EHB10:EHP21 EQX10:ERL21 FAT10:FBH21 FKP10:FLD21 FUL10:FUZ21 GEH10:GEV21 GOD10:GOR21 GXZ10:GYN21 HHV10:HIJ21 HRR10:HSF21 IBN10:ICB21 ILJ10:ILX21 IVF10:IVT21 JFB10:JFP21 JOX10:JPL21 JYT10:JZH21 KIP10:KJD21 KSL10:KSZ21 LCH10:LCV21 LMD10:LMR21 LVZ10:LWN21 MFV10:MGJ21 MPR10:MQF21 MZN10:NAB21 NJJ10:NJX21 NTF10:NTT21 ODB10:ODP21 OMX10:ONL21 OWT10:OXH21 PGP10:PHD21 PQL10:PQZ21 QAH10:QAV21 QKD10:QKR21 QTZ10:QUN21 RDV10:REJ21 RNR10:ROF21 RXN10:RYB21 SHJ10:SHX21 SRF10:SRT21 TBB10:TBP21 TKX10:TLL21 TUT10:TVH21 UEP10:UFD21 UOL10:UOZ21 UYH10:UYV21 VID10:VIR21 VRZ10:VSN21 WBV10:WCJ21 WLR10:WMF21 WVN10:WWB21 F65546:T65557 JB65546:JP65557 SX65546:TL65557 ACT65546:ADH65557 AMP65546:AND65557 AWL65546:AWZ65557 BGH65546:BGV65557 BQD65546:BQR65557 BZZ65546:CAN65557 CJV65546:CKJ65557 CTR65546:CUF65557 DDN65546:DEB65557 DNJ65546:DNX65557 DXF65546:DXT65557 EHB65546:EHP65557 EQX65546:ERL65557 FAT65546:FBH65557 FKP65546:FLD65557 FUL65546:FUZ65557 GEH65546:GEV65557 GOD65546:GOR65557 GXZ65546:GYN65557 HHV65546:HIJ65557 HRR65546:HSF65557 IBN65546:ICB65557 ILJ65546:ILX65557 IVF65546:IVT65557 JFB65546:JFP65557 JOX65546:JPL65557 JYT65546:JZH65557 KIP65546:KJD65557 KSL65546:KSZ65557 LCH65546:LCV65557 LMD65546:LMR65557 LVZ65546:LWN65557 MFV65546:MGJ65557 MPR65546:MQF65557 MZN65546:NAB65557 NJJ65546:NJX65557 NTF65546:NTT65557 ODB65546:ODP65557 OMX65546:ONL65557 OWT65546:OXH65557 PGP65546:PHD65557 PQL65546:PQZ65557 QAH65546:QAV65557 QKD65546:QKR65557 QTZ65546:QUN65557 RDV65546:REJ65557 RNR65546:ROF65557 RXN65546:RYB65557 SHJ65546:SHX65557 SRF65546:SRT65557 TBB65546:TBP65557 TKX65546:TLL65557 TUT65546:TVH65557 UEP65546:UFD65557 UOL65546:UOZ65557 UYH65546:UYV65557 VID65546:VIR65557 VRZ65546:VSN65557 WBV65546:WCJ65557 WLR65546:WMF65557 WVN65546:WWB65557 F131082:T131093 JB131082:JP131093 SX131082:TL131093 ACT131082:ADH131093 AMP131082:AND131093 AWL131082:AWZ131093 BGH131082:BGV131093 BQD131082:BQR131093 BZZ131082:CAN131093 CJV131082:CKJ131093 CTR131082:CUF131093 DDN131082:DEB131093 DNJ131082:DNX131093 DXF131082:DXT131093 EHB131082:EHP131093 EQX131082:ERL131093 FAT131082:FBH131093 FKP131082:FLD131093 FUL131082:FUZ131093 GEH131082:GEV131093 GOD131082:GOR131093 GXZ131082:GYN131093 HHV131082:HIJ131093 HRR131082:HSF131093 IBN131082:ICB131093 ILJ131082:ILX131093 IVF131082:IVT131093 JFB131082:JFP131093 JOX131082:JPL131093 JYT131082:JZH131093 KIP131082:KJD131093 KSL131082:KSZ131093 LCH131082:LCV131093 LMD131082:LMR131093 LVZ131082:LWN131093 MFV131082:MGJ131093 MPR131082:MQF131093 MZN131082:NAB131093 NJJ131082:NJX131093 NTF131082:NTT131093 ODB131082:ODP131093 OMX131082:ONL131093 OWT131082:OXH131093 PGP131082:PHD131093 PQL131082:PQZ131093 QAH131082:QAV131093 QKD131082:QKR131093 QTZ131082:QUN131093 RDV131082:REJ131093 RNR131082:ROF131093 RXN131082:RYB131093 SHJ131082:SHX131093 SRF131082:SRT131093 TBB131082:TBP131093 TKX131082:TLL131093 TUT131082:TVH131093 UEP131082:UFD131093 UOL131082:UOZ131093 UYH131082:UYV131093 VID131082:VIR131093 VRZ131082:VSN131093 WBV131082:WCJ131093 WLR131082:WMF131093 WVN131082:WWB131093 F196618:T196629 JB196618:JP196629 SX196618:TL196629 ACT196618:ADH196629 AMP196618:AND196629 AWL196618:AWZ196629 BGH196618:BGV196629 BQD196618:BQR196629 BZZ196618:CAN196629 CJV196618:CKJ196629 CTR196618:CUF196629 DDN196618:DEB196629 DNJ196618:DNX196629 DXF196618:DXT196629 EHB196618:EHP196629 EQX196618:ERL196629 FAT196618:FBH196629 FKP196618:FLD196629 FUL196618:FUZ196629 GEH196618:GEV196629 GOD196618:GOR196629 GXZ196618:GYN196629 HHV196618:HIJ196629 HRR196618:HSF196629 IBN196618:ICB196629 ILJ196618:ILX196629 IVF196618:IVT196629 JFB196618:JFP196629 JOX196618:JPL196629 JYT196618:JZH196629 KIP196618:KJD196629 KSL196618:KSZ196629 LCH196618:LCV196629 LMD196618:LMR196629 LVZ196618:LWN196629 MFV196618:MGJ196629 MPR196618:MQF196629 MZN196618:NAB196629 NJJ196618:NJX196629 NTF196618:NTT196629 ODB196618:ODP196629 OMX196618:ONL196629 OWT196618:OXH196629 PGP196618:PHD196629 PQL196618:PQZ196629 QAH196618:QAV196629 QKD196618:QKR196629 QTZ196618:QUN196629 RDV196618:REJ196629 RNR196618:ROF196629 RXN196618:RYB196629 SHJ196618:SHX196629 SRF196618:SRT196629 TBB196618:TBP196629 TKX196618:TLL196629 TUT196618:TVH196629 UEP196618:UFD196629 UOL196618:UOZ196629 UYH196618:UYV196629 VID196618:VIR196629 VRZ196618:VSN196629 WBV196618:WCJ196629 WLR196618:WMF196629 WVN196618:WWB196629 F262154:T262165 JB262154:JP262165 SX262154:TL262165 ACT262154:ADH262165 AMP262154:AND262165 AWL262154:AWZ262165 BGH262154:BGV262165 BQD262154:BQR262165 BZZ262154:CAN262165 CJV262154:CKJ262165 CTR262154:CUF262165 DDN262154:DEB262165 DNJ262154:DNX262165 DXF262154:DXT262165 EHB262154:EHP262165 EQX262154:ERL262165 FAT262154:FBH262165 FKP262154:FLD262165 FUL262154:FUZ262165 GEH262154:GEV262165 GOD262154:GOR262165 GXZ262154:GYN262165 HHV262154:HIJ262165 HRR262154:HSF262165 IBN262154:ICB262165 ILJ262154:ILX262165 IVF262154:IVT262165 JFB262154:JFP262165 JOX262154:JPL262165 JYT262154:JZH262165 KIP262154:KJD262165 KSL262154:KSZ262165 LCH262154:LCV262165 LMD262154:LMR262165 LVZ262154:LWN262165 MFV262154:MGJ262165 MPR262154:MQF262165 MZN262154:NAB262165 NJJ262154:NJX262165 NTF262154:NTT262165 ODB262154:ODP262165 OMX262154:ONL262165 OWT262154:OXH262165 PGP262154:PHD262165 PQL262154:PQZ262165 QAH262154:QAV262165 QKD262154:QKR262165 QTZ262154:QUN262165 RDV262154:REJ262165 RNR262154:ROF262165 RXN262154:RYB262165 SHJ262154:SHX262165 SRF262154:SRT262165 TBB262154:TBP262165 TKX262154:TLL262165 TUT262154:TVH262165 UEP262154:UFD262165 UOL262154:UOZ262165 UYH262154:UYV262165 VID262154:VIR262165 VRZ262154:VSN262165 WBV262154:WCJ262165 WLR262154:WMF262165 WVN262154:WWB262165 F327690:T327701 JB327690:JP327701 SX327690:TL327701 ACT327690:ADH327701 AMP327690:AND327701 AWL327690:AWZ327701 BGH327690:BGV327701 BQD327690:BQR327701 BZZ327690:CAN327701 CJV327690:CKJ327701 CTR327690:CUF327701 DDN327690:DEB327701 DNJ327690:DNX327701 DXF327690:DXT327701 EHB327690:EHP327701 EQX327690:ERL327701 FAT327690:FBH327701 FKP327690:FLD327701 FUL327690:FUZ327701 GEH327690:GEV327701 GOD327690:GOR327701 GXZ327690:GYN327701 HHV327690:HIJ327701 HRR327690:HSF327701 IBN327690:ICB327701 ILJ327690:ILX327701 IVF327690:IVT327701 JFB327690:JFP327701 JOX327690:JPL327701 JYT327690:JZH327701 KIP327690:KJD327701 KSL327690:KSZ327701 LCH327690:LCV327701 LMD327690:LMR327701 LVZ327690:LWN327701 MFV327690:MGJ327701 MPR327690:MQF327701 MZN327690:NAB327701 NJJ327690:NJX327701 NTF327690:NTT327701 ODB327690:ODP327701 OMX327690:ONL327701 OWT327690:OXH327701 PGP327690:PHD327701 PQL327690:PQZ327701 QAH327690:QAV327701 QKD327690:QKR327701 QTZ327690:QUN327701 RDV327690:REJ327701 RNR327690:ROF327701 RXN327690:RYB327701 SHJ327690:SHX327701 SRF327690:SRT327701 TBB327690:TBP327701 TKX327690:TLL327701 TUT327690:TVH327701 UEP327690:UFD327701 UOL327690:UOZ327701 UYH327690:UYV327701 VID327690:VIR327701 VRZ327690:VSN327701 WBV327690:WCJ327701 WLR327690:WMF327701 WVN327690:WWB327701 F393226:T393237 JB393226:JP393237 SX393226:TL393237 ACT393226:ADH393237 AMP393226:AND393237 AWL393226:AWZ393237 BGH393226:BGV393237 BQD393226:BQR393237 BZZ393226:CAN393237 CJV393226:CKJ393237 CTR393226:CUF393237 DDN393226:DEB393237 DNJ393226:DNX393237 DXF393226:DXT393237 EHB393226:EHP393237 EQX393226:ERL393237 FAT393226:FBH393237 FKP393226:FLD393237 FUL393226:FUZ393237 GEH393226:GEV393237 GOD393226:GOR393237 GXZ393226:GYN393237 HHV393226:HIJ393237 HRR393226:HSF393237 IBN393226:ICB393237 ILJ393226:ILX393237 IVF393226:IVT393237 JFB393226:JFP393237 JOX393226:JPL393237 JYT393226:JZH393237 KIP393226:KJD393237 KSL393226:KSZ393237 LCH393226:LCV393237 LMD393226:LMR393237 LVZ393226:LWN393237 MFV393226:MGJ393237 MPR393226:MQF393237 MZN393226:NAB393237 NJJ393226:NJX393237 NTF393226:NTT393237 ODB393226:ODP393237 OMX393226:ONL393237 OWT393226:OXH393237 PGP393226:PHD393237 PQL393226:PQZ393237 QAH393226:QAV393237 QKD393226:QKR393237 QTZ393226:QUN393237 RDV393226:REJ393237 RNR393226:ROF393237 RXN393226:RYB393237 SHJ393226:SHX393237 SRF393226:SRT393237 TBB393226:TBP393237 TKX393226:TLL393237 TUT393226:TVH393237 UEP393226:UFD393237 UOL393226:UOZ393237 UYH393226:UYV393237 VID393226:VIR393237 VRZ393226:VSN393237 WBV393226:WCJ393237 WLR393226:WMF393237 WVN393226:WWB393237 F458762:T458773 JB458762:JP458773 SX458762:TL458773 ACT458762:ADH458773 AMP458762:AND458773 AWL458762:AWZ458773 BGH458762:BGV458773 BQD458762:BQR458773 BZZ458762:CAN458773 CJV458762:CKJ458773 CTR458762:CUF458773 DDN458762:DEB458773 DNJ458762:DNX458773 DXF458762:DXT458773 EHB458762:EHP458773 EQX458762:ERL458773 FAT458762:FBH458773 FKP458762:FLD458773 FUL458762:FUZ458773 GEH458762:GEV458773 GOD458762:GOR458773 GXZ458762:GYN458773 HHV458762:HIJ458773 HRR458762:HSF458773 IBN458762:ICB458773 ILJ458762:ILX458773 IVF458762:IVT458773 JFB458762:JFP458773 JOX458762:JPL458773 JYT458762:JZH458773 KIP458762:KJD458773 KSL458762:KSZ458773 LCH458762:LCV458773 LMD458762:LMR458773 LVZ458762:LWN458773 MFV458762:MGJ458773 MPR458762:MQF458773 MZN458762:NAB458773 NJJ458762:NJX458773 NTF458762:NTT458773 ODB458762:ODP458773 OMX458762:ONL458773 OWT458762:OXH458773 PGP458762:PHD458773 PQL458762:PQZ458773 QAH458762:QAV458773 QKD458762:QKR458773 QTZ458762:QUN458773 RDV458762:REJ458773 RNR458762:ROF458773 RXN458762:RYB458773 SHJ458762:SHX458773 SRF458762:SRT458773 TBB458762:TBP458773 TKX458762:TLL458773 TUT458762:TVH458773 UEP458762:UFD458773 UOL458762:UOZ458773 UYH458762:UYV458773 VID458762:VIR458773 VRZ458762:VSN458773 WBV458762:WCJ458773 WLR458762:WMF458773 WVN458762:WWB458773 F524298:T524309 JB524298:JP524309 SX524298:TL524309 ACT524298:ADH524309 AMP524298:AND524309 AWL524298:AWZ524309 BGH524298:BGV524309 BQD524298:BQR524309 BZZ524298:CAN524309 CJV524298:CKJ524309 CTR524298:CUF524309 DDN524298:DEB524309 DNJ524298:DNX524309 DXF524298:DXT524309 EHB524298:EHP524309 EQX524298:ERL524309 FAT524298:FBH524309 FKP524298:FLD524309 FUL524298:FUZ524309 GEH524298:GEV524309 GOD524298:GOR524309 GXZ524298:GYN524309 HHV524298:HIJ524309 HRR524298:HSF524309 IBN524298:ICB524309 ILJ524298:ILX524309 IVF524298:IVT524309 JFB524298:JFP524309 JOX524298:JPL524309 JYT524298:JZH524309 KIP524298:KJD524309 KSL524298:KSZ524309 LCH524298:LCV524309 LMD524298:LMR524309 LVZ524298:LWN524309 MFV524298:MGJ524309 MPR524298:MQF524309 MZN524298:NAB524309 NJJ524298:NJX524309 NTF524298:NTT524309 ODB524298:ODP524309 OMX524298:ONL524309 OWT524298:OXH524309 PGP524298:PHD524309 PQL524298:PQZ524309 QAH524298:QAV524309 QKD524298:QKR524309 QTZ524298:QUN524309 RDV524298:REJ524309 RNR524298:ROF524309 RXN524298:RYB524309 SHJ524298:SHX524309 SRF524298:SRT524309 TBB524298:TBP524309 TKX524298:TLL524309 TUT524298:TVH524309 UEP524298:UFD524309 UOL524298:UOZ524309 UYH524298:UYV524309 VID524298:VIR524309 VRZ524298:VSN524309 WBV524298:WCJ524309 WLR524298:WMF524309 WVN524298:WWB524309 F589834:T589845 JB589834:JP589845 SX589834:TL589845 ACT589834:ADH589845 AMP589834:AND589845 AWL589834:AWZ589845 BGH589834:BGV589845 BQD589834:BQR589845 BZZ589834:CAN589845 CJV589834:CKJ589845 CTR589834:CUF589845 DDN589834:DEB589845 DNJ589834:DNX589845 DXF589834:DXT589845 EHB589834:EHP589845 EQX589834:ERL589845 FAT589834:FBH589845 FKP589834:FLD589845 FUL589834:FUZ589845 GEH589834:GEV589845 GOD589834:GOR589845 GXZ589834:GYN589845 HHV589834:HIJ589845 HRR589834:HSF589845 IBN589834:ICB589845 ILJ589834:ILX589845 IVF589834:IVT589845 JFB589834:JFP589845 JOX589834:JPL589845 JYT589834:JZH589845 KIP589834:KJD589845 KSL589834:KSZ589845 LCH589834:LCV589845 LMD589834:LMR589845 LVZ589834:LWN589845 MFV589834:MGJ589845 MPR589834:MQF589845 MZN589834:NAB589845 NJJ589834:NJX589845 NTF589834:NTT589845 ODB589834:ODP589845 OMX589834:ONL589845 OWT589834:OXH589845 PGP589834:PHD589845 PQL589834:PQZ589845 QAH589834:QAV589845 QKD589834:QKR589845 QTZ589834:QUN589845 RDV589834:REJ589845 RNR589834:ROF589845 RXN589834:RYB589845 SHJ589834:SHX589845 SRF589834:SRT589845 TBB589834:TBP589845 TKX589834:TLL589845 TUT589834:TVH589845 UEP589834:UFD589845 UOL589834:UOZ589845 UYH589834:UYV589845 VID589834:VIR589845 VRZ589834:VSN589845 WBV589834:WCJ589845 WLR589834:WMF589845 WVN589834:WWB589845 F655370:T655381 JB655370:JP655381 SX655370:TL655381 ACT655370:ADH655381 AMP655370:AND655381 AWL655370:AWZ655381 BGH655370:BGV655381 BQD655370:BQR655381 BZZ655370:CAN655381 CJV655370:CKJ655381 CTR655370:CUF655381 DDN655370:DEB655381 DNJ655370:DNX655381 DXF655370:DXT655381 EHB655370:EHP655381 EQX655370:ERL655381 FAT655370:FBH655381 FKP655370:FLD655381 FUL655370:FUZ655381 GEH655370:GEV655381 GOD655370:GOR655381 GXZ655370:GYN655381 HHV655370:HIJ655381 HRR655370:HSF655381 IBN655370:ICB655381 ILJ655370:ILX655381 IVF655370:IVT655381 JFB655370:JFP655381 JOX655370:JPL655381 JYT655370:JZH655381 KIP655370:KJD655381 KSL655370:KSZ655381 LCH655370:LCV655381 LMD655370:LMR655381 LVZ655370:LWN655381 MFV655370:MGJ655381 MPR655370:MQF655381 MZN655370:NAB655381 NJJ655370:NJX655381 NTF655370:NTT655381 ODB655370:ODP655381 OMX655370:ONL655381 OWT655370:OXH655381 PGP655370:PHD655381 PQL655370:PQZ655381 QAH655370:QAV655381 QKD655370:QKR655381 QTZ655370:QUN655381 RDV655370:REJ655381 RNR655370:ROF655381 RXN655370:RYB655381 SHJ655370:SHX655381 SRF655370:SRT655381 TBB655370:TBP655381 TKX655370:TLL655381 TUT655370:TVH655381 UEP655370:UFD655381 UOL655370:UOZ655381 UYH655370:UYV655381 VID655370:VIR655381 VRZ655370:VSN655381 WBV655370:WCJ655381 WLR655370:WMF655381 WVN655370:WWB655381 F720906:T720917 JB720906:JP720917 SX720906:TL720917 ACT720906:ADH720917 AMP720906:AND720917 AWL720906:AWZ720917 BGH720906:BGV720917 BQD720906:BQR720917 BZZ720906:CAN720917 CJV720906:CKJ720917 CTR720906:CUF720917 DDN720906:DEB720917 DNJ720906:DNX720917 DXF720906:DXT720917 EHB720906:EHP720917 EQX720906:ERL720917 FAT720906:FBH720917 FKP720906:FLD720917 FUL720906:FUZ720917 GEH720906:GEV720917 GOD720906:GOR720917 GXZ720906:GYN720917 HHV720906:HIJ720917 HRR720906:HSF720917 IBN720906:ICB720917 ILJ720906:ILX720917 IVF720906:IVT720917 JFB720906:JFP720917 JOX720906:JPL720917 JYT720906:JZH720917 KIP720906:KJD720917 KSL720906:KSZ720917 LCH720906:LCV720917 LMD720906:LMR720917 LVZ720906:LWN720917 MFV720906:MGJ720917 MPR720906:MQF720917 MZN720906:NAB720917 NJJ720906:NJX720917 NTF720906:NTT720917 ODB720906:ODP720917 OMX720906:ONL720917 OWT720906:OXH720917 PGP720906:PHD720917 PQL720906:PQZ720917 QAH720906:QAV720917 QKD720906:QKR720917 QTZ720906:QUN720917 RDV720906:REJ720917 RNR720906:ROF720917 RXN720906:RYB720917 SHJ720906:SHX720917 SRF720906:SRT720917 TBB720906:TBP720917 TKX720906:TLL720917 TUT720906:TVH720917 UEP720906:UFD720917 UOL720906:UOZ720917 UYH720906:UYV720917 VID720906:VIR720917 VRZ720906:VSN720917 WBV720906:WCJ720917 WLR720906:WMF720917 WVN720906:WWB720917 F786442:T786453 JB786442:JP786453 SX786442:TL786453 ACT786442:ADH786453 AMP786442:AND786453 AWL786442:AWZ786453 BGH786442:BGV786453 BQD786442:BQR786453 BZZ786442:CAN786453 CJV786442:CKJ786453 CTR786442:CUF786453 DDN786442:DEB786453 DNJ786442:DNX786453 DXF786442:DXT786453 EHB786442:EHP786453 EQX786442:ERL786453 FAT786442:FBH786453 FKP786442:FLD786453 FUL786442:FUZ786453 GEH786442:GEV786453 GOD786442:GOR786453 GXZ786442:GYN786453 HHV786442:HIJ786453 HRR786442:HSF786453 IBN786442:ICB786453 ILJ786442:ILX786453 IVF786442:IVT786453 JFB786442:JFP786453 JOX786442:JPL786453 JYT786442:JZH786453 KIP786442:KJD786453 KSL786442:KSZ786453 LCH786442:LCV786453 LMD786442:LMR786453 LVZ786442:LWN786453 MFV786442:MGJ786453 MPR786442:MQF786453 MZN786442:NAB786453 NJJ786442:NJX786453 NTF786442:NTT786453 ODB786442:ODP786453 OMX786442:ONL786453 OWT786442:OXH786453 PGP786442:PHD786453 PQL786442:PQZ786453 QAH786442:QAV786453 QKD786442:QKR786453 QTZ786442:QUN786453 RDV786442:REJ786453 RNR786442:ROF786453 RXN786442:RYB786453 SHJ786442:SHX786453 SRF786442:SRT786453 TBB786442:TBP786453 TKX786442:TLL786453 TUT786442:TVH786453 UEP786442:UFD786453 UOL786442:UOZ786453 UYH786442:UYV786453 VID786442:VIR786453 VRZ786442:VSN786453 WBV786442:WCJ786453 WLR786442:WMF786453 WVN786442:WWB786453 F851978:T851989 JB851978:JP851989 SX851978:TL851989 ACT851978:ADH851989 AMP851978:AND851989 AWL851978:AWZ851989 BGH851978:BGV851989 BQD851978:BQR851989 BZZ851978:CAN851989 CJV851978:CKJ851989 CTR851978:CUF851989 DDN851978:DEB851989 DNJ851978:DNX851989 DXF851978:DXT851989 EHB851978:EHP851989 EQX851978:ERL851989 FAT851978:FBH851989 FKP851978:FLD851989 FUL851978:FUZ851989 GEH851978:GEV851989 GOD851978:GOR851989 GXZ851978:GYN851989 HHV851978:HIJ851989 HRR851978:HSF851989 IBN851978:ICB851989 ILJ851978:ILX851989 IVF851978:IVT851989 JFB851978:JFP851989 JOX851978:JPL851989 JYT851978:JZH851989 KIP851978:KJD851989 KSL851978:KSZ851989 LCH851978:LCV851989 LMD851978:LMR851989 LVZ851978:LWN851989 MFV851978:MGJ851989 MPR851978:MQF851989 MZN851978:NAB851989 NJJ851978:NJX851989 NTF851978:NTT851989 ODB851978:ODP851989 OMX851978:ONL851989 OWT851978:OXH851989 PGP851978:PHD851989 PQL851978:PQZ851989 QAH851978:QAV851989 QKD851978:QKR851989 QTZ851978:QUN851989 RDV851978:REJ851989 RNR851978:ROF851989 RXN851978:RYB851989 SHJ851978:SHX851989 SRF851978:SRT851989 TBB851978:TBP851989 TKX851978:TLL851989 TUT851978:TVH851989 UEP851978:UFD851989 UOL851978:UOZ851989 UYH851978:UYV851989 VID851978:VIR851989 VRZ851978:VSN851989 WBV851978:WCJ851989 WLR851978:WMF851989 WVN851978:WWB851989 F917514:T917525 JB917514:JP917525 SX917514:TL917525 ACT917514:ADH917525 AMP917514:AND917525 AWL917514:AWZ917525 BGH917514:BGV917525 BQD917514:BQR917525 BZZ917514:CAN917525 CJV917514:CKJ917525 CTR917514:CUF917525 DDN917514:DEB917525 DNJ917514:DNX917525 DXF917514:DXT917525 EHB917514:EHP917525 EQX917514:ERL917525 FAT917514:FBH917525 FKP917514:FLD917525 FUL917514:FUZ917525 GEH917514:GEV917525 GOD917514:GOR917525 GXZ917514:GYN917525 HHV917514:HIJ917525 HRR917514:HSF917525 IBN917514:ICB917525 ILJ917514:ILX917525 IVF917514:IVT917525 JFB917514:JFP917525 JOX917514:JPL917525 JYT917514:JZH917525 KIP917514:KJD917525 KSL917514:KSZ917525 LCH917514:LCV917525 LMD917514:LMR917525 LVZ917514:LWN917525 MFV917514:MGJ917525 MPR917514:MQF917525 MZN917514:NAB917525 NJJ917514:NJX917525 NTF917514:NTT917525 ODB917514:ODP917525 OMX917514:ONL917525 OWT917514:OXH917525 PGP917514:PHD917525 PQL917514:PQZ917525 QAH917514:QAV917525 QKD917514:QKR917525 QTZ917514:QUN917525 RDV917514:REJ917525 RNR917514:ROF917525 RXN917514:RYB917525 SHJ917514:SHX917525 SRF917514:SRT917525 TBB917514:TBP917525 TKX917514:TLL917525 TUT917514:TVH917525 UEP917514:UFD917525 UOL917514:UOZ917525 UYH917514:UYV917525 VID917514:VIR917525 VRZ917514:VSN917525 WBV917514:WCJ917525 WLR917514:WMF917525 WVN917514:WWB917525 F983050:T983061 JB983050:JP983061 SX983050:TL983061 ACT983050:ADH983061 AMP983050:AND983061 AWL983050:AWZ983061 BGH983050:BGV983061 BQD983050:BQR983061 BZZ983050:CAN983061 CJV983050:CKJ983061 CTR983050:CUF983061 DDN983050:DEB983061 DNJ983050:DNX983061 DXF983050:DXT983061 EHB983050:EHP983061 EQX983050:ERL983061 FAT983050:FBH983061 FKP983050:FLD983061 FUL983050:FUZ983061 GEH983050:GEV983061 GOD983050:GOR983061 GXZ983050:GYN983061 HHV983050:HIJ983061 HRR983050:HSF983061 IBN983050:ICB983061 ILJ983050:ILX983061 IVF983050:IVT983061 JFB983050:JFP983061 JOX983050:JPL983061 JYT983050:JZH983061 KIP983050:KJD983061 KSL983050:KSZ983061 LCH983050:LCV983061 LMD983050:LMR983061 LVZ983050:LWN983061 MFV983050:MGJ983061 MPR983050:MQF983061 MZN983050:NAB983061 NJJ983050:NJX983061 NTF983050:NTT983061 ODB983050:ODP983061 OMX983050:ONL983061 OWT983050:OXH983061 PGP983050:PHD983061 PQL983050:PQZ983061 QAH983050:QAV983061 QKD983050:QKR983061 QTZ983050:QUN983061 RDV983050:REJ983061 RNR983050:ROF983061 RXN983050:RYB983061 SHJ983050:SHX983061 SRF983050:SRT983061 TBB983050:TBP983061 TKX983050:TLL983061 TUT983050:TVH983061 UEP983050:UFD983061 UOL983050:UOZ983061 UYH983050:UYV983061 VID983050:VIR983061 VRZ983050:VSN983061 WBV983050:WCJ983061 WLR983050:WMF983061 WVN983050:WWB983061">
@@ -4555,51 +4555,51 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:26">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="93"/>
-      <c r="F2" s="94" t="s">
+      <c r="B2" s="64"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="66"/>
+      <c r="F2" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="96"/>
-      <c r="S2" s="96"/>
-      <c r="T2" s="97"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="69"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="69"/>
+      <c r="T2" s="70"/>
     </row>
     <row r="3" spans="1:26">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="98" t="s">
+      <c r="B3" s="72"/>
+      <c r="C3" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="99"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="82" t="s">
+      <c r="D3" s="74"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="88"/>
-      <c r="N3" s="88"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
@@ -4608,112 +4608,112 @@
       <c r="T3" s="6"/>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="79"/>
+      <c r="B4" s="72"/>
       <c r="C4" s="80"/>
       <c r="D4" s="81"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="82" t="s">
+      <c r="F4" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="84"/>
-      <c r="M4" s="85"/>
-      <c r="N4" s="85"/>
-      <c r="O4" s="85"/>
-      <c r="P4" s="85"/>
-      <c r="Q4" s="85"/>
-      <c r="R4" s="85"/>
-      <c r="S4" s="85"/>
-      <c r="T4" s="86"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="83"/>
+      <c r="P4" s="83"/>
+      <c r="Q4" s="83"/>
+      <c r="R4" s="83"/>
+      <c r="S4" s="83"/>
+      <c r="T4" s="84"/>
       <c r="V4" s="8"/>
     </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="87" t="s">
+      <c r="B5" s="72"/>
+      <c r="C5" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="88"/>
-      <c r="K5" s="88"/>
-      <c r="L5" s="88"/>
-      <c r="M5" s="88"/>
-      <c r="N5" s="88"/>
-      <c r="O5" s="88"/>
-      <c r="P5" s="88"/>
-      <c r="Q5" s="88"/>
-      <c r="R5" s="88"/>
-      <c r="S5" s="88"/>
-      <c r="T5" s="89"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="79"/>
+      <c r="Q5" s="79"/>
+      <c r="R5" s="79"/>
+      <c r="S5" s="79"/>
+      <c r="T5" s="85"/>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="69" t="s">
+      <c r="B6" s="100"/>
+      <c r="C6" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="70"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="69" t="s">
+      <c r="D6" s="87"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="69" t="s">
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="88"/>
+      <c r="L6" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="70"/>
-      <c r="N6" s="71"/>
-      <c r="O6" s="69" t="s">
+      <c r="M6" s="87"/>
+      <c r="N6" s="88"/>
+      <c r="O6" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="70"/>
-      <c r="Q6" s="70"/>
-      <c r="R6" s="70"/>
-      <c r="S6" s="70"/>
-      <c r="T6" s="72"/>
+      <c r="P6" s="87"/>
+      <c r="Q6" s="87"/>
+      <c r="R6" s="87"/>
+      <c r="S6" s="87"/>
+      <c r="T6" s="89"/>
       <c r="V6" s="8"/>
     </row>
     <row r="7" spans="1:26" ht="11.25" thickBot="1">
-      <c r="A7" s="73">
+      <c r="A7" s="90">
         <f>COUNTIF(F23:HQ23,"P")</f>
         <v>2</v>
       </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="75">
+      <c r="B7" s="91"/>
+      <c r="C7" s="92">
         <f>COUNTIF(F23:HQ23,"F")</f>
         <v>0</v>
       </c>
-      <c r="D7" s="76"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="75">
+      <c r="D7" s="93"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="92">
         <f>SUM(O7,-A7,-C7)</f>
         <v>19</v>
       </c>
-      <c r="G7" s="76"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="76"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="74"/>
+      <c r="G7" s="93"/>
+      <c r="H7" s="93"/>
+      <c r="I7" s="93"/>
+      <c r="J7" s="93"/>
+      <c r="K7" s="91"/>
       <c r="L7" s="9">
         <f>COUNTIF(E22:HQ22,"N")</f>
         <v>0</v>
@@ -4726,15 +4726,15 @@
         <f>COUNTIF(E22:HQ22,"B")</f>
         <v>0</v>
       </c>
-      <c r="O7" s="75">
+      <c r="O7" s="92">
         <f>COUNTA(E9:HT9)</f>
         <v>21</v>
       </c>
-      <c r="P7" s="76"/>
-      <c r="Q7" s="76"/>
-      <c r="R7" s="76"/>
-      <c r="S7" s="76"/>
-      <c r="T7" s="77"/>
+      <c r="P7" s="93"/>
+      <c r="Q7" s="93"/>
+      <c r="R7" s="93"/>
+      <c r="S7" s="93"/>
+      <c r="T7" s="94"/>
       <c r="U7" s="10"/>
     </row>
     <row r="8" spans="1:26" ht="11.25" thickBot="1"/>
@@ -5176,11 +5176,11 @@
       <c r="A22" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="63" t="s">
+      <c r="B22" s="95" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="95"/>
       <c r="E22" s="49"/>
       <c r="F22" s="50"/>
       <c r="G22" s="50"/>
@@ -5206,11 +5206,11 @@
     </row>
     <row r="23" spans="1:26" ht="11.25">
       <c r="A23" s="52"/>
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="96" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="96"/>
       <c r="E23" s="53"/>
       <c r="F23" s="54" t="s">
         <v>46</v>
@@ -5240,11 +5240,11 @@
     </row>
     <row r="24" spans="1:26">
       <c r="A24" s="52"/>
-      <c r="B24" s="65" t="s">
+      <c r="B24" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
+      <c r="C24" s="97"/>
+      <c r="D24" s="97"/>
       <c r="E24" s="56"/>
       <c r="F24" s="57"/>
       <c r="G24" s="57"/>
@@ -5270,11 +5270,11 @@
     </row>
     <row r="25" spans="1:26" ht="11.25" thickBot="1">
       <c r="A25" s="59"/>
-      <c r="B25" s="66" t="s">
+      <c r="B25" s="98" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="66"/>
-      <c r="D25" s="66"/>
+      <c r="C25" s="98"/>
+      <c r="D25" s="98"/>
       <c r="E25" s="60"/>
       <c r="F25" s="61"/>
       <c r="G25" s="61"/>
@@ -5306,6 +5306,25 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:K6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="O6:T6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:K7"/>
+    <mergeCell ref="O7:T7"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="L4:T4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:T5"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:K2"/>
@@ -5314,25 +5333,6 @@
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="F3:K3"/>
     <mergeCell ref="L3:N3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:K4"/>
-    <mergeCell ref="L4:T4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:T5"/>
-    <mergeCell ref="F6:K6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="O6:T6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:K7"/>
-    <mergeCell ref="O7:T7"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F10:T21 JB10:JP21 SX10:TL21 ACT10:ADH21 AMP10:AND21 AWL10:AWZ21 BGH10:BGV21 BQD10:BQR21 BZZ10:CAN21 CJV10:CKJ21 CTR10:CUF21 DDN10:DEB21 DNJ10:DNX21 DXF10:DXT21 EHB10:EHP21 EQX10:ERL21 FAT10:FBH21 FKP10:FLD21 FUL10:FUZ21 GEH10:GEV21 GOD10:GOR21 GXZ10:GYN21 HHV10:HIJ21 HRR10:HSF21 IBN10:ICB21 ILJ10:ILX21 IVF10:IVT21 JFB10:JFP21 JOX10:JPL21 JYT10:JZH21 KIP10:KJD21 KSL10:KSZ21 LCH10:LCV21 LMD10:LMR21 LVZ10:LWN21 MFV10:MGJ21 MPR10:MQF21 MZN10:NAB21 NJJ10:NJX21 NTF10:NTT21 ODB10:ODP21 OMX10:ONL21 OWT10:OXH21 PGP10:PHD21 PQL10:PQZ21 QAH10:QAV21 QKD10:QKR21 QTZ10:QUN21 RDV10:REJ21 RNR10:ROF21 RXN10:RYB21 SHJ10:SHX21 SRF10:SRT21 TBB10:TBP21 TKX10:TLL21 TUT10:TVH21 UEP10:UFD21 UOL10:UOZ21 UYH10:UYV21 VID10:VIR21 VRZ10:VSN21 WBV10:WCJ21 WLR10:WMF21 WVN10:WWB21 F65546:T65557 JB65546:JP65557 SX65546:TL65557 ACT65546:ADH65557 AMP65546:AND65557 AWL65546:AWZ65557 BGH65546:BGV65557 BQD65546:BQR65557 BZZ65546:CAN65557 CJV65546:CKJ65557 CTR65546:CUF65557 DDN65546:DEB65557 DNJ65546:DNX65557 DXF65546:DXT65557 EHB65546:EHP65557 EQX65546:ERL65557 FAT65546:FBH65557 FKP65546:FLD65557 FUL65546:FUZ65557 GEH65546:GEV65557 GOD65546:GOR65557 GXZ65546:GYN65557 HHV65546:HIJ65557 HRR65546:HSF65557 IBN65546:ICB65557 ILJ65546:ILX65557 IVF65546:IVT65557 JFB65546:JFP65557 JOX65546:JPL65557 JYT65546:JZH65557 KIP65546:KJD65557 KSL65546:KSZ65557 LCH65546:LCV65557 LMD65546:LMR65557 LVZ65546:LWN65557 MFV65546:MGJ65557 MPR65546:MQF65557 MZN65546:NAB65557 NJJ65546:NJX65557 NTF65546:NTT65557 ODB65546:ODP65557 OMX65546:ONL65557 OWT65546:OXH65557 PGP65546:PHD65557 PQL65546:PQZ65557 QAH65546:QAV65557 QKD65546:QKR65557 QTZ65546:QUN65557 RDV65546:REJ65557 RNR65546:ROF65557 RXN65546:RYB65557 SHJ65546:SHX65557 SRF65546:SRT65557 TBB65546:TBP65557 TKX65546:TLL65557 TUT65546:TVH65557 UEP65546:UFD65557 UOL65546:UOZ65557 UYH65546:UYV65557 VID65546:VIR65557 VRZ65546:VSN65557 WBV65546:WCJ65557 WLR65546:WMF65557 WVN65546:WWB65557 F131082:T131093 JB131082:JP131093 SX131082:TL131093 ACT131082:ADH131093 AMP131082:AND131093 AWL131082:AWZ131093 BGH131082:BGV131093 BQD131082:BQR131093 BZZ131082:CAN131093 CJV131082:CKJ131093 CTR131082:CUF131093 DDN131082:DEB131093 DNJ131082:DNX131093 DXF131082:DXT131093 EHB131082:EHP131093 EQX131082:ERL131093 FAT131082:FBH131093 FKP131082:FLD131093 FUL131082:FUZ131093 GEH131082:GEV131093 GOD131082:GOR131093 GXZ131082:GYN131093 HHV131082:HIJ131093 HRR131082:HSF131093 IBN131082:ICB131093 ILJ131082:ILX131093 IVF131082:IVT131093 JFB131082:JFP131093 JOX131082:JPL131093 JYT131082:JZH131093 KIP131082:KJD131093 KSL131082:KSZ131093 LCH131082:LCV131093 LMD131082:LMR131093 LVZ131082:LWN131093 MFV131082:MGJ131093 MPR131082:MQF131093 MZN131082:NAB131093 NJJ131082:NJX131093 NTF131082:NTT131093 ODB131082:ODP131093 OMX131082:ONL131093 OWT131082:OXH131093 PGP131082:PHD131093 PQL131082:PQZ131093 QAH131082:QAV131093 QKD131082:QKR131093 QTZ131082:QUN131093 RDV131082:REJ131093 RNR131082:ROF131093 RXN131082:RYB131093 SHJ131082:SHX131093 SRF131082:SRT131093 TBB131082:TBP131093 TKX131082:TLL131093 TUT131082:TVH131093 UEP131082:UFD131093 UOL131082:UOZ131093 UYH131082:UYV131093 VID131082:VIR131093 VRZ131082:VSN131093 WBV131082:WCJ131093 WLR131082:WMF131093 WVN131082:WWB131093 F196618:T196629 JB196618:JP196629 SX196618:TL196629 ACT196618:ADH196629 AMP196618:AND196629 AWL196618:AWZ196629 BGH196618:BGV196629 BQD196618:BQR196629 BZZ196618:CAN196629 CJV196618:CKJ196629 CTR196618:CUF196629 DDN196618:DEB196629 DNJ196618:DNX196629 DXF196618:DXT196629 EHB196618:EHP196629 EQX196618:ERL196629 FAT196618:FBH196629 FKP196618:FLD196629 FUL196618:FUZ196629 GEH196618:GEV196629 GOD196618:GOR196629 GXZ196618:GYN196629 HHV196618:HIJ196629 HRR196618:HSF196629 IBN196618:ICB196629 ILJ196618:ILX196629 IVF196618:IVT196629 JFB196618:JFP196629 JOX196618:JPL196629 JYT196618:JZH196629 KIP196618:KJD196629 KSL196618:KSZ196629 LCH196618:LCV196629 LMD196618:LMR196629 LVZ196618:LWN196629 MFV196618:MGJ196629 MPR196618:MQF196629 MZN196618:NAB196629 NJJ196618:NJX196629 NTF196618:NTT196629 ODB196618:ODP196629 OMX196618:ONL196629 OWT196618:OXH196629 PGP196618:PHD196629 PQL196618:PQZ196629 QAH196618:QAV196629 QKD196618:QKR196629 QTZ196618:QUN196629 RDV196618:REJ196629 RNR196618:ROF196629 RXN196618:RYB196629 SHJ196618:SHX196629 SRF196618:SRT196629 TBB196618:TBP196629 TKX196618:TLL196629 TUT196618:TVH196629 UEP196618:UFD196629 UOL196618:UOZ196629 UYH196618:UYV196629 VID196618:VIR196629 VRZ196618:VSN196629 WBV196618:WCJ196629 WLR196618:WMF196629 WVN196618:WWB196629 F262154:T262165 JB262154:JP262165 SX262154:TL262165 ACT262154:ADH262165 AMP262154:AND262165 AWL262154:AWZ262165 BGH262154:BGV262165 BQD262154:BQR262165 BZZ262154:CAN262165 CJV262154:CKJ262165 CTR262154:CUF262165 DDN262154:DEB262165 DNJ262154:DNX262165 DXF262154:DXT262165 EHB262154:EHP262165 EQX262154:ERL262165 FAT262154:FBH262165 FKP262154:FLD262165 FUL262154:FUZ262165 GEH262154:GEV262165 GOD262154:GOR262165 GXZ262154:GYN262165 HHV262154:HIJ262165 HRR262154:HSF262165 IBN262154:ICB262165 ILJ262154:ILX262165 IVF262154:IVT262165 JFB262154:JFP262165 JOX262154:JPL262165 JYT262154:JZH262165 KIP262154:KJD262165 KSL262154:KSZ262165 LCH262154:LCV262165 LMD262154:LMR262165 LVZ262154:LWN262165 MFV262154:MGJ262165 MPR262154:MQF262165 MZN262154:NAB262165 NJJ262154:NJX262165 NTF262154:NTT262165 ODB262154:ODP262165 OMX262154:ONL262165 OWT262154:OXH262165 PGP262154:PHD262165 PQL262154:PQZ262165 QAH262154:QAV262165 QKD262154:QKR262165 QTZ262154:QUN262165 RDV262154:REJ262165 RNR262154:ROF262165 RXN262154:RYB262165 SHJ262154:SHX262165 SRF262154:SRT262165 TBB262154:TBP262165 TKX262154:TLL262165 TUT262154:TVH262165 UEP262154:UFD262165 UOL262154:UOZ262165 UYH262154:UYV262165 VID262154:VIR262165 VRZ262154:VSN262165 WBV262154:WCJ262165 WLR262154:WMF262165 WVN262154:WWB262165 F327690:T327701 JB327690:JP327701 SX327690:TL327701 ACT327690:ADH327701 AMP327690:AND327701 AWL327690:AWZ327701 BGH327690:BGV327701 BQD327690:BQR327701 BZZ327690:CAN327701 CJV327690:CKJ327701 CTR327690:CUF327701 DDN327690:DEB327701 DNJ327690:DNX327701 DXF327690:DXT327701 EHB327690:EHP327701 EQX327690:ERL327701 FAT327690:FBH327701 FKP327690:FLD327701 FUL327690:FUZ327701 GEH327690:GEV327701 GOD327690:GOR327701 GXZ327690:GYN327701 HHV327690:HIJ327701 HRR327690:HSF327701 IBN327690:ICB327701 ILJ327690:ILX327701 IVF327690:IVT327701 JFB327690:JFP327701 JOX327690:JPL327701 JYT327690:JZH327701 KIP327690:KJD327701 KSL327690:KSZ327701 LCH327690:LCV327701 LMD327690:LMR327701 LVZ327690:LWN327701 MFV327690:MGJ327701 MPR327690:MQF327701 MZN327690:NAB327701 NJJ327690:NJX327701 NTF327690:NTT327701 ODB327690:ODP327701 OMX327690:ONL327701 OWT327690:OXH327701 PGP327690:PHD327701 PQL327690:PQZ327701 QAH327690:QAV327701 QKD327690:QKR327701 QTZ327690:QUN327701 RDV327690:REJ327701 RNR327690:ROF327701 RXN327690:RYB327701 SHJ327690:SHX327701 SRF327690:SRT327701 TBB327690:TBP327701 TKX327690:TLL327701 TUT327690:TVH327701 UEP327690:UFD327701 UOL327690:UOZ327701 UYH327690:UYV327701 VID327690:VIR327701 VRZ327690:VSN327701 WBV327690:WCJ327701 WLR327690:WMF327701 WVN327690:WWB327701 F393226:T393237 JB393226:JP393237 SX393226:TL393237 ACT393226:ADH393237 AMP393226:AND393237 AWL393226:AWZ393237 BGH393226:BGV393237 BQD393226:BQR393237 BZZ393226:CAN393237 CJV393226:CKJ393237 CTR393226:CUF393237 DDN393226:DEB393237 DNJ393226:DNX393237 DXF393226:DXT393237 EHB393226:EHP393237 EQX393226:ERL393237 FAT393226:FBH393237 FKP393226:FLD393237 FUL393226:FUZ393237 GEH393226:GEV393237 GOD393226:GOR393237 GXZ393226:GYN393237 HHV393226:HIJ393237 HRR393226:HSF393237 IBN393226:ICB393237 ILJ393226:ILX393237 IVF393226:IVT393237 JFB393226:JFP393237 JOX393226:JPL393237 JYT393226:JZH393237 KIP393226:KJD393237 KSL393226:KSZ393237 LCH393226:LCV393237 LMD393226:LMR393237 LVZ393226:LWN393237 MFV393226:MGJ393237 MPR393226:MQF393237 MZN393226:NAB393237 NJJ393226:NJX393237 NTF393226:NTT393237 ODB393226:ODP393237 OMX393226:ONL393237 OWT393226:OXH393237 PGP393226:PHD393237 PQL393226:PQZ393237 QAH393226:QAV393237 QKD393226:QKR393237 QTZ393226:QUN393237 RDV393226:REJ393237 RNR393226:ROF393237 RXN393226:RYB393237 SHJ393226:SHX393237 SRF393226:SRT393237 TBB393226:TBP393237 TKX393226:TLL393237 TUT393226:TVH393237 UEP393226:UFD393237 UOL393226:UOZ393237 UYH393226:UYV393237 VID393226:VIR393237 VRZ393226:VSN393237 WBV393226:WCJ393237 WLR393226:WMF393237 WVN393226:WWB393237 F458762:T458773 JB458762:JP458773 SX458762:TL458773 ACT458762:ADH458773 AMP458762:AND458773 AWL458762:AWZ458773 BGH458762:BGV458773 BQD458762:BQR458773 BZZ458762:CAN458773 CJV458762:CKJ458773 CTR458762:CUF458773 DDN458762:DEB458773 DNJ458762:DNX458773 DXF458762:DXT458773 EHB458762:EHP458773 EQX458762:ERL458773 FAT458762:FBH458773 FKP458762:FLD458773 FUL458762:FUZ458773 GEH458762:GEV458773 GOD458762:GOR458773 GXZ458762:GYN458773 HHV458762:HIJ458773 HRR458762:HSF458773 IBN458762:ICB458773 ILJ458762:ILX458773 IVF458762:IVT458773 JFB458762:JFP458773 JOX458762:JPL458773 JYT458762:JZH458773 KIP458762:KJD458773 KSL458762:KSZ458773 LCH458762:LCV458773 LMD458762:LMR458773 LVZ458762:LWN458773 MFV458762:MGJ458773 MPR458762:MQF458773 MZN458762:NAB458773 NJJ458762:NJX458773 NTF458762:NTT458773 ODB458762:ODP458773 OMX458762:ONL458773 OWT458762:OXH458773 PGP458762:PHD458773 PQL458762:PQZ458773 QAH458762:QAV458773 QKD458762:QKR458773 QTZ458762:QUN458773 RDV458762:REJ458773 RNR458762:ROF458773 RXN458762:RYB458773 SHJ458762:SHX458773 SRF458762:SRT458773 TBB458762:TBP458773 TKX458762:TLL458773 TUT458762:TVH458773 UEP458762:UFD458773 UOL458762:UOZ458773 UYH458762:UYV458773 VID458762:VIR458773 VRZ458762:VSN458773 WBV458762:WCJ458773 WLR458762:WMF458773 WVN458762:WWB458773 F524298:T524309 JB524298:JP524309 SX524298:TL524309 ACT524298:ADH524309 AMP524298:AND524309 AWL524298:AWZ524309 BGH524298:BGV524309 BQD524298:BQR524309 BZZ524298:CAN524309 CJV524298:CKJ524309 CTR524298:CUF524309 DDN524298:DEB524309 DNJ524298:DNX524309 DXF524298:DXT524309 EHB524298:EHP524309 EQX524298:ERL524309 FAT524298:FBH524309 FKP524298:FLD524309 FUL524298:FUZ524309 GEH524298:GEV524309 GOD524298:GOR524309 GXZ524298:GYN524309 HHV524298:HIJ524309 HRR524298:HSF524309 IBN524298:ICB524309 ILJ524298:ILX524309 IVF524298:IVT524309 JFB524298:JFP524309 JOX524298:JPL524309 JYT524298:JZH524309 KIP524298:KJD524309 KSL524298:KSZ524309 LCH524298:LCV524309 LMD524298:LMR524309 LVZ524298:LWN524309 MFV524298:MGJ524309 MPR524298:MQF524309 MZN524298:NAB524309 NJJ524298:NJX524309 NTF524298:NTT524309 ODB524298:ODP524309 OMX524298:ONL524309 OWT524298:OXH524309 PGP524298:PHD524309 PQL524298:PQZ524309 QAH524298:QAV524309 QKD524298:QKR524309 QTZ524298:QUN524309 RDV524298:REJ524309 RNR524298:ROF524309 RXN524298:RYB524309 SHJ524298:SHX524309 SRF524298:SRT524309 TBB524298:TBP524309 TKX524298:TLL524309 TUT524298:TVH524309 UEP524298:UFD524309 UOL524298:UOZ524309 UYH524298:UYV524309 VID524298:VIR524309 VRZ524298:VSN524309 WBV524298:WCJ524309 WLR524298:WMF524309 WVN524298:WWB524309 F589834:T589845 JB589834:JP589845 SX589834:TL589845 ACT589834:ADH589845 AMP589834:AND589845 AWL589834:AWZ589845 BGH589834:BGV589845 BQD589834:BQR589845 BZZ589834:CAN589845 CJV589834:CKJ589845 CTR589834:CUF589845 DDN589834:DEB589845 DNJ589834:DNX589845 DXF589834:DXT589845 EHB589834:EHP589845 EQX589834:ERL589845 FAT589834:FBH589845 FKP589834:FLD589845 FUL589834:FUZ589845 GEH589834:GEV589845 GOD589834:GOR589845 GXZ589834:GYN589845 HHV589834:HIJ589845 HRR589834:HSF589845 IBN589834:ICB589845 ILJ589834:ILX589845 IVF589834:IVT589845 JFB589834:JFP589845 JOX589834:JPL589845 JYT589834:JZH589845 KIP589834:KJD589845 KSL589834:KSZ589845 LCH589834:LCV589845 LMD589834:LMR589845 LVZ589834:LWN589845 MFV589834:MGJ589845 MPR589834:MQF589845 MZN589834:NAB589845 NJJ589834:NJX589845 NTF589834:NTT589845 ODB589834:ODP589845 OMX589834:ONL589845 OWT589834:OXH589845 PGP589834:PHD589845 PQL589834:PQZ589845 QAH589834:QAV589845 QKD589834:QKR589845 QTZ589834:QUN589845 RDV589834:REJ589845 RNR589834:ROF589845 RXN589834:RYB589845 SHJ589834:SHX589845 SRF589834:SRT589845 TBB589834:TBP589845 TKX589834:TLL589845 TUT589834:TVH589845 UEP589834:UFD589845 UOL589834:UOZ589845 UYH589834:UYV589845 VID589834:VIR589845 VRZ589834:VSN589845 WBV589834:WCJ589845 WLR589834:WMF589845 WVN589834:WWB589845 F655370:T655381 JB655370:JP655381 SX655370:TL655381 ACT655370:ADH655381 AMP655370:AND655381 AWL655370:AWZ655381 BGH655370:BGV655381 BQD655370:BQR655381 BZZ655370:CAN655381 CJV655370:CKJ655381 CTR655370:CUF655381 DDN655370:DEB655381 DNJ655370:DNX655381 DXF655370:DXT655381 EHB655370:EHP655381 EQX655370:ERL655381 FAT655370:FBH655381 FKP655370:FLD655381 FUL655370:FUZ655381 GEH655370:GEV655381 GOD655370:GOR655381 GXZ655370:GYN655381 HHV655370:HIJ655381 HRR655370:HSF655381 IBN655370:ICB655381 ILJ655370:ILX655381 IVF655370:IVT655381 JFB655370:JFP655381 JOX655370:JPL655381 JYT655370:JZH655381 KIP655370:KJD655381 KSL655370:KSZ655381 LCH655370:LCV655381 LMD655370:LMR655381 LVZ655370:LWN655381 MFV655370:MGJ655381 MPR655370:MQF655381 MZN655370:NAB655381 NJJ655370:NJX655381 NTF655370:NTT655381 ODB655370:ODP655381 OMX655370:ONL655381 OWT655370:OXH655381 PGP655370:PHD655381 PQL655370:PQZ655381 QAH655370:QAV655381 QKD655370:QKR655381 QTZ655370:QUN655381 RDV655370:REJ655381 RNR655370:ROF655381 RXN655370:RYB655381 SHJ655370:SHX655381 SRF655370:SRT655381 TBB655370:TBP655381 TKX655370:TLL655381 TUT655370:TVH655381 UEP655370:UFD655381 UOL655370:UOZ655381 UYH655370:UYV655381 VID655370:VIR655381 VRZ655370:VSN655381 WBV655370:WCJ655381 WLR655370:WMF655381 WVN655370:WWB655381 F720906:T720917 JB720906:JP720917 SX720906:TL720917 ACT720906:ADH720917 AMP720906:AND720917 AWL720906:AWZ720917 BGH720906:BGV720917 BQD720906:BQR720917 BZZ720906:CAN720917 CJV720906:CKJ720917 CTR720906:CUF720917 DDN720906:DEB720917 DNJ720906:DNX720917 DXF720906:DXT720917 EHB720906:EHP720917 EQX720906:ERL720917 FAT720906:FBH720917 FKP720906:FLD720917 FUL720906:FUZ720917 GEH720906:GEV720917 GOD720906:GOR720917 GXZ720906:GYN720917 HHV720906:HIJ720917 HRR720906:HSF720917 IBN720906:ICB720917 ILJ720906:ILX720917 IVF720906:IVT720917 JFB720906:JFP720917 JOX720906:JPL720917 JYT720906:JZH720917 KIP720906:KJD720917 KSL720906:KSZ720917 LCH720906:LCV720917 LMD720906:LMR720917 LVZ720906:LWN720917 MFV720906:MGJ720917 MPR720906:MQF720917 MZN720906:NAB720917 NJJ720906:NJX720917 NTF720906:NTT720917 ODB720906:ODP720917 OMX720906:ONL720917 OWT720906:OXH720917 PGP720906:PHD720917 PQL720906:PQZ720917 QAH720906:QAV720917 QKD720906:QKR720917 QTZ720906:QUN720917 RDV720906:REJ720917 RNR720906:ROF720917 RXN720906:RYB720917 SHJ720906:SHX720917 SRF720906:SRT720917 TBB720906:TBP720917 TKX720906:TLL720917 TUT720906:TVH720917 UEP720906:UFD720917 UOL720906:UOZ720917 UYH720906:UYV720917 VID720906:VIR720917 VRZ720906:VSN720917 WBV720906:WCJ720917 WLR720906:WMF720917 WVN720906:WWB720917 F786442:T786453 JB786442:JP786453 SX786442:TL786453 ACT786442:ADH786453 AMP786442:AND786453 AWL786442:AWZ786453 BGH786442:BGV786453 BQD786442:BQR786453 BZZ786442:CAN786453 CJV786442:CKJ786453 CTR786442:CUF786453 DDN786442:DEB786453 DNJ786442:DNX786453 DXF786442:DXT786453 EHB786442:EHP786453 EQX786442:ERL786453 FAT786442:FBH786453 FKP786442:FLD786453 FUL786442:FUZ786453 GEH786442:GEV786453 GOD786442:GOR786453 GXZ786442:GYN786453 HHV786442:HIJ786453 HRR786442:HSF786453 IBN786442:ICB786453 ILJ786442:ILX786453 IVF786442:IVT786453 JFB786442:JFP786453 JOX786442:JPL786453 JYT786442:JZH786453 KIP786442:KJD786453 KSL786442:KSZ786453 LCH786442:LCV786453 LMD786442:LMR786453 LVZ786442:LWN786453 MFV786442:MGJ786453 MPR786442:MQF786453 MZN786442:NAB786453 NJJ786442:NJX786453 NTF786442:NTT786453 ODB786442:ODP786453 OMX786442:ONL786453 OWT786442:OXH786453 PGP786442:PHD786453 PQL786442:PQZ786453 QAH786442:QAV786453 QKD786442:QKR786453 QTZ786442:QUN786453 RDV786442:REJ786453 RNR786442:ROF786453 RXN786442:RYB786453 SHJ786442:SHX786453 SRF786442:SRT786453 TBB786442:TBP786453 TKX786442:TLL786453 TUT786442:TVH786453 UEP786442:UFD786453 UOL786442:UOZ786453 UYH786442:UYV786453 VID786442:VIR786453 VRZ786442:VSN786453 WBV786442:WCJ786453 WLR786442:WMF786453 WVN786442:WWB786453 F851978:T851989 JB851978:JP851989 SX851978:TL851989 ACT851978:ADH851989 AMP851978:AND851989 AWL851978:AWZ851989 BGH851978:BGV851989 BQD851978:BQR851989 BZZ851978:CAN851989 CJV851978:CKJ851989 CTR851978:CUF851989 DDN851978:DEB851989 DNJ851978:DNX851989 DXF851978:DXT851989 EHB851978:EHP851989 EQX851978:ERL851989 FAT851978:FBH851989 FKP851978:FLD851989 FUL851978:FUZ851989 GEH851978:GEV851989 GOD851978:GOR851989 GXZ851978:GYN851989 HHV851978:HIJ851989 HRR851978:HSF851989 IBN851978:ICB851989 ILJ851978:ILX851989 IVF851978:IVT851989 JFB851978:JFP851989 JOX851978:JPL851989 JYT851978:JZH851989 KIP851978:KJD851989 KSL851978:KSZ851989 LCH851978:LCV851989 LMD851978:LMR851989 LVZ851978:LWN851989 MFV851978:MGJ851989 MPR851978:MQF851989 MZN851978:NAB851989 NJJ851978:NJX851989 NTF851978:NTT851989 ODB851978:ODP851989 OMX851978:ONL851989 OWT851978:OXH851989 PGP851978:PHD851989 PQL851978:PQZ851989 QAH851978:QAV851989 QKD851978:QKR851989 QTZ851978:QUN851989 RDV851978:REJ851989 RNR851978:ROF851989 RXN851978:RYB851989 SHJ851978:SHX851989 SRF851978:SRT851989 TBB851978:TBP851989 TKX851978:TLL851989 TUT851978:TVH851989 UEP851978:UFD851989 UOL851978:UOZ851989 UYH851978:UYV851989 VID851978:VIR851989 VRZ851978:VSN851989 WBV851978:WCJ851989 WLR851978:WMF851989 WVN851978:WWB851989 F917514:T917525 JB917514:JP917525 SX917514:TL917525 ACT917514:ADH917525 AMP917514:AND917525 AWL917514:AWZ917525 BGH917514:BGV917525 BQD917514:BQR917525 BZZ917514:CAN917525 CJV917514:CKJ917525 CTR917514:CUF917525 DDN917514:DEB917525 DNJ917514:DNX917525 DXF917514:DXT917525 EHB917514:EHP917525 EQX917514:ERL917525 FAT917514:FBH917525 FKP917514:FLD917525 FUL917514:FUZ917525 GEH917514:GEV917525 GOD917514:GOR917525 GXZ917514:GYN917525 HHV917514:HIJ917525 HRR917514:HSF917525 IBN917514:ICB917525 ILJ917514:ILX917525 IVF917514:IVT917525 JFB917514:JFP917525 JOX917514:JPL917525 JYT917514:JZH917525 KIP917514:KJD917525 KSL917514:KSZ917525 LCH917514:LCV917525 LMD917514:LMR917525 LVZ917514:LWN917525 MFV917514:MGJ917525 MPR917514:MQF917525 MZN917514:NAB917525 NJJ917514:NJX917525 NTF917514:NTT917525 ODB917514:ODP917525 OMX917514:ONL917525 OWT917514:OXH917525 PGP917514:PHD917525 PQL917514:PQZ917525 QAH917514:QAV917525 QKD917514:QKR917525 QTZ917514:QUN917525 RDV917514:REJ917525 RNR917514:ROF917525 RXN917514:RYB917525 SHJ917514:SHX917525 SRF917514:SRT917525 TBB917514:TBP917525 TKX917514:TLL917525 TUT917514:TVH917525 UEP917514:UFD917525 UOL917514:UOZ917525 UYH917514:UYV917525 VID917514:VIR917525 VRZ917514:VSN917525 WBV917514:WCJ917525 WLR917514:WMF917525 WVN917514:WWB917525 F983050:T983061 JB983050:JP983061 SX983050:TL983061 ACT983050:ADH983061 AMP983050:AND983061 AWL983050:AWZ983061 BGH983050:BGV983061 BQD983050:BQR983061 BZZ983050:CAN983061 CJV983050:CKJ983061 CTR983050:CUF983061 DDN983050:DEB983061 DNJ983050:DNX983061 DXF983050:DXT983061 EHB983050:EHP983061 EQX983050:ERL983061 FAT983050:FBH983061 FKP983050:FLD983061 FUL983050:FUZ983061 GEH983050:GEV983061 GOD983050:GOR983061 GXZ983050:GYN983061 HHV983050:HIJ983061 HRR983050:HSF983061 IBN983050:ICB983061 ILJ983050:ILX983061 IVF983050:IVT983061 JFB983050:JFP983061 JOX983050:JPL983061 JYT983050:JZH983061 KIP983050:KJD983061 KSL983050:KSZ983061 LCH983050:LCV983061 LMD983050:LMR983061 LVZ983050:LWN983061 MFV983050:MGJ983061 MPR983050:MQF983061 MZN983050:NAB983061 NJJ983050:NJX983061 NTF983050:NTT983061 ODB983050:ODP983061 OMX983050:ONL983061 OWT983050:OXH983061 PGP983050:PHD983061 PQL983050:PQZ983061 QAH983050:QAV983061 QKD983050:QKR983061 QTZ983050:QUN983061 RDV983050:REJ983061 RNR983050:ROF983061 RXN983050:RYB983061 SHJ983050:SHX983061 SRF983050:SRT983061 TBB983050:TBP983061 TKX983050:TLL983061 TUT983050:TVH983061 UEP983050:UFD983061 UOL983050:UOZ983061 UYH983050:UYV983061 VID983050:VIR983061 VRZ983050:VSN983061 WBV983050:WCJ983061 WLR983050:WMF983061 WVN983050:WWB983061">
@@ -5818,51 +5818,51 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:26">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="93"/>
-      <c r="F2" s="94" t="s">
+      <c r="B2" s="64"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="66"/>
+      <c r="F2" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="96"/>
-      <c r="S2" s="96"/>
-      <c r="T2" s="97"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="69"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="69"/>
+      <c r="T2" s="70"/>
     </row>
     <row r="3" spans="1:26">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="98" t="s">
+      <c r="B3" s="72"/>
+      <c r="C3" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="99"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="82" t="s">
+      <c r="D3" s="74"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="88"/>
-      <c r="N3" s="88"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
@@ -5871,112 +5871,112 @@
       <c r="T3" s="6"/>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="79"/>
+      <c r="B4" s="72"/>
       <c r="C4" s="80"/>
       <c r="D4" s="81"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="82" t="s">
+      <c r="F4" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="84"/>
-      <c r="M4" s="85"/>
-      <c r="N4" s="85"/>
-      <c r="O4" s="85"/>
-      <c r="P4" s="85"/>
-      <c r="Q4" s="85"/>
-      <c r="R4" s="85"/>
-      <c r="S4" s="85"/>
-      <c r="T4" s="86"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="83"/>
+      <c r="P4" s="83"/>
+      <c r="Q4" s="83"/>
+      <c r="R4" s="83"/>
+      <c r="S4" s="83"/>
+      <c r="T4" s="84"/>
       <c r="V4" s="8"/>
     </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="87" t="s">
+      <c r="B5" s="72"/>
+      <c r="C5" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="88"/>
-      <c r="K5" s="88"/>
-      <c r="L5" s="88"/>
-      <c r="M5" s="88"/>
-      <c r="N5" s="88"/>
-      <c r="O5" s="88"/>
-      <c r="P5" s="88"/>
-      <c r="Q5" s="88"/>
-      <c r="R5" s="88"/>
-      <c r="S5" s="88"/>
-      <c r="T5" s="89"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="79"/>
+      <c r="Q5" s="79"/>
+      <c r="R5" s="79"/>
+      <c r="S5" s="79"/>
+      <c r="T5" s="85"/>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="69" t="s">
+      <c r="B6" s="100"/>
+      <c r="C6" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="70"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="69" t="s">
+      <c r="D6" s="87"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="69" t="s">
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="88"/>
+      <c r="L6" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="70"/>
-      <c r="N6" s="71"/>
-      <c r="O6" s="69" t="s">
+      <c r="M6" s="87"/>
+      <c r="N6" s="88"/>
+      <c r="O6" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="70"/>
-      <c r="Q6" s="70"/>
-      <c r="R6" s="70"/>
-      <c r="S6" s="70"/>
-      <c r="T6" s="72"/>
+      <c r="P6" s="87"/>
+      <c r="Q6" s="87"/>
+      <c r="R6" s="87"/>
+      <c r="S6" s="87"/>
+      <c r="T6" s="89"/>
       <c r="V6" s="8"/>
     </row>
     <row r="7" spans="1:26" ht="11.25" thickBot="1">
-      <c r="A7" s="73">
+      <c r="A7" s="90">
         <f>COUNTIF(F23:HQ23,"P")</f>
         <v>4</v>
       </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="75">
+      <c r="B7" s="91"/>
+      <c r="C7" s="92">
         <f>COUNTIF(F23:HQ23,"F")</f>
         <v>0</v>
       </c>
-      <c r="D7" s="76"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="75">
+      <c r="D7" s="93"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="92">
         <f>SUM(O7,-A7,-C7)</f>
         <v>17</v>
       </c>
-      <c r="G7" s="76"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="76"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="74"/>
+      <c r="G7" s="93"/>
+      <c r="H7" s="93"/>
+      <c r="I7" s="93"/>
+      <c r="J7" s="93"/>
+      <c r="K7" s="91"/>
       <c r="L7" s="9">
         <f>COUNTIF(E22:HQ22,"N")</f>
         <v>0</v>
@@ -5989,15 +5989,15 @@
         <f>COUNTIF(E22:HQ22,"B")</f>
         <v>0</v>
       </c>
-      <c r="O7" s="75">
+      <c r="O7" s="92">
         <f>COUNTA(E9:HT9)</f>
         <v>21</v>
       </c>
-      <c r="P7" s="76"/>
-      <c r="Q7" s="76"/>
-      <c r="R7" s="76"/>
-      <c r="S7" s="76"/>
-      <c r="T7" s="77"/>
+      <c r="P7" s="93"/>
+      <c r="Q7" s="93"/>
+      <c r="R7" s="93"/>
+      <c r="S7" s="93"/>
+      <c r="T7" s="94"/>
       <c r="U7" s="10"/>
     </row>
     <row r="8" spans="1:26" ht="11.25" thickBot="1"/>
@@ -6080,7 +6080,7 @@
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E10" s="22"/>
       <c r="F10" s="23" t="s">
@@ -6112,7 +6112,7 @@
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
       <c r="D11" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E11" s="26"/>
       <c r="F11" s="23"/>
@@ -6176,7 +6176,7 @@
       <c r="B13" s="19"/>
       <c r="C13" s="20"/>
       <c r="D13" s="21" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E13" s="27"/>
       <c r="F13" s="23"/>
@@ -6451,11 +6451,11 @@
       <c r="A22" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="63" t="s">
+      <c r="B22" s="95" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="95"/>
       <c r="E22" s="49"/>
       <c r="F22" s="50"/>
       <c r="G22" s="50"/>
@@ -6481,11 +6481,11 @@
     </row>
     <row r="23" spans="1:26" ht="11.25">
       <c r="A23" s="52"/>
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="96" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="96"/>
       <c r="E23" s="53"/>
       <c r="F23" s="54" t="s">
         <v>46</v>
@@ -6519,11 +6519,11 @@
     </row>
     <row r="24" spans="1:26">
       <c r="A24" s="52"/>
-      <c r="B24" s="65" t="s">
+      <c r="B24" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
+      <c r="C24" s="97"/>
+      <c r="D24" s="97"/>
       <c r="E24" s="56"/>
       <c r="F24" s="57"/>
       <c r="G24" s="57"/>
@@ -6549,11 +6549,11 @@
     </row>
     <row r="25" spans="1:26" ht="11.25" thickBot="1">
       <c r="A25" s="59"/>
-      <c r="B25" s="66" t="s">
+      <c r="B25" s="98" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="66"/>
-      <c r="D25" s="66"/>
+      <c r="C25" s="98"/>
+      <c r="D25" s="98"/>
       <c r="E25" s="60"/>
       <c r="F25" s="61"/>
       <c r="G25" s="61"/>
@@ -6585,6 +6585,25 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:K6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="O6:T6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:K7"/>
+    <mergeCell ref="O7:T7"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="L4:T4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:T5"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:K2"/>
@@ -6593,25 +6612,6 @@
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="F3:K3"/>
     <mergeCell ref="L3:N3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:K4"/>
-    <mergeCell ref="L4:T4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:T5"/>
-    <mergeCell ref="F6:K6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="O6:T6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:K7"/>
-    <mergeCell ref="O7:T7"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F22:T22 JB22:JP22 SX22:TL22 ACT22:ADH22 AMP22:AND22 AWL22:AWZ22 BGH22:BGV22 BQD22:BQR22 BZZ22:CAN22 CJV22:CKJ22 CTR22:CUF22 DDN22:DEB22 DNJ22:DNX22 DXF22:DXT22 EHB22:EHP22 EQX22:ERL22 FAT22:FBH22 FKP22:FLD22 FUL22:FUZ22 GEH22:GEV22 GOD22:GOR22 GXZ22:GYN22 HHV22:HIJ22 HRR22:HSF22 IBN22:ICB22 ILJ22:ILX22 IVF22:IVT22 JFB22:JFP22 JOX22:JPL22 JYT22:JZH22 KIP22:KJD22 KSL22:KSZ22 LCH22:LCV22 LMD22:LMR22 LVZ22:LWN22 MFV22:MGJ22 MPR22:MQF22 MZN22:NAB22 NJJ22:NJX22 NTF22:NTT22 ODB22:ODP22 OMX22:ONL22 OWT22:OXH22 PGP22:PHD22 PQL22:PQZ22 QAH22:QAV22 QKD22:QKR22 QTZ22:QUN22 RDV22:REJ22 RNR22:ROF22 RXN22:RYB22 SHJ22:SHX22 SRF22:SRT22 TBB22:TBP22 TKX22:TLL22 TUT22:TVH22 UEP22:UFD22 UOL22:UOZ22 UYH22:UYV22 VID22:VIR22 VRZ22:VSN22 WBV22:WCJ22 WLR22:WMF22 WVN22:WWB22 F65558:T65558 JB65558:JP65558 SX65558:TL65558 ACT65558:ADH65558 AMP65558:AND65558 AWL65558:AWZ65558 BGH65558:BGV65558 BQD65558:BQR65558 BZZ65558:CAN65558 CJV65558:CKJ65558 CTR65558:CUF65558 DDN65558:DEB65558 DNJ65558:DNX65558 DXF65558:DXT65558 EHB65558:EHP65558 EQX65558:ERL65558 FAT65558:FBH65558 FKP65558:FLD65558 FUL65558:FUZ65558 GEH65558:GEV65558 GOD65558:GOR65558 GXZ65558:GYN65558 HHV65558:HIJ65558 HRR65558:HSF65558 IBN65558:ICB65558 ILJ65558:ILX65558 IVF65558:IVT65558 JFB65558:JFP65558 JOX65558:JPL65558 JYT65558:JZH65558 KIP65558:KJD65558 KSL65558:KSZ65558 LCH65558:LCV65558 LMD65558:LMR65558 LVZ65558:LWN65558 MFV65558:MGJ65558 MPR65558:MQF65558 MZN65558:NAB65558 NJJ65558:NJX65558 NTF65558:NTT65558 ODB65558:ODP65558 OMX65558:ONL65558 OWT65558:OXH65558 PGP65558:PHD65558 PQL65558:PQZ65558 QAH65558:QAV65558 QKD65558:QKR65558 QTZ65558:QUN65558 RDV65558:REJ65558 RNR65558:ROF65558 RXN65558:RYB65558 SHJ65558:SHX65558 SRF65558:SRT65558 TBB65558:TBP65558 TKX65558:TLL65558 TUT65558:TVH65558 UEP65558:UFD65558 UOL65558:UOZ65558 UYH65558:UYV65558 VID65558:VIR65558 VRZ65558:VSN65558 WBV65558:WCJ65558 WLR65558:WMF65558 WVN65558:WWB65558 F131094:T131094 JB131094:JP131094 SX131094:TL131094 ACT131094:ADH131094 AMP131094:AND131094 AWL131094:AWZ131094 BGH131094:BGV131094 BQD131094:BQR131094 BZZ131094:CAN131094 CJV131094:CKJ131094 CTR131094:CUF131094 DDN131094:DEB131094 DNJ131094:DNX131094 DXF131094:DXT131094 EHB131094:EHP131094 EQX131094:ERL131094 FAT131094:FBH131094 FKP131094:FLD131094 FUL131094:FUZ131094 GEH131094:GEV131094 GOD131094:GOR131094 GXZ131094:GYN131094 HHV131094:HIJ131094 HRR131094:HSF131094 IBN131094:ICB131094 ILJ131094:ILX131094 IVF131094:IVT131094 JFB131094:JFP131094 JOX131094:JPL131094 JYT131094:JZH131094 KIP131094:KJD131094 KSL131094:KSZ131094 LCH131094:LCV131094 LMD131094:LMR131094 LVZ131094:LWN131094 MFV131094:MGJ131094 MPR131094:MQF131094 MZN131094:NAB131094 NJJ131094:NJX131094 NTF131094:NTT131094 ODB131094:ODP131094 OMX131094:ONL131094 OWT131094:OXH131094 PGP131094:PHD131094 PQL131094:PQZ131094 QAH131094:QAV131094 QKD131094:QKR131094 QTZ131094:QUN131094 RDV131094:REJ131094 RNR131094:ROF131094 RXN131094:RYB131094 SHJ131094:SHX131094 SRF131094:SRT131094 TBB131094:TBP131094 TKX131094:TLL131094 TUT131094:TVH131094 UEP131094:UFD131094 UOL131094:UOZ131094 UYH131094:UYV131094 VID131094:VIR131094 VRZ131094:VSN131094 WBV131094:WCJ131094 WLR131094:WMF131094 WVN131094:WWB131094 F196630:T196630 JB196630:JP196630 SX196630:TL196630 ACT196630:ADH196630 AMP196630:AND196630 AWL196630:AWZ196630 BGH196630:BGV196630 BQD196630:BQR196630 BZZ196630:CAN196630 CJV196630:CKJ196630 CTR196630:CUF196630 DDN196630:DEB196630 DNJ196630:DNX196630 DXF196630:DXT196630 EHB196630:EHP196630 EQX196630:ERL196630 FAT196630:FBH196630 FKP196630:FLD196630 FUL196630:FUZ196630 GEH196630:GEV196630 GOD196630:GOR196630 GXZ196630:GYN196630 HHV196630:HIJ196630 HRR196630:HSF196630 IBN196630:ICB196630 ILJ196630:ILX196630 IVF196630:IVT196630 JFB196630:JFP196630 JOX196630:JPL196630 JYT196630:JZH196630 KIP196630:KJD196630 KSL196630:KSZ196630 LCH196630:LCV196630 LMD196630:LMR196630 LVZ196630:LWN196630 MFV196630:MGJ196630 MPR196630:MQF196630 MZN196630:NAB196630 NJJ196630:NJX196630 NTF196630:NTT196630 ODB196630:ODP196630 OMX196630:ONL196630 OWT196630:OXH196630 PGP196630:PHD196630 PQL196630:PQZ196630 QAH196630:QAV196630 QKD196630:QKR196630 QTZ196630:QUN196630 RDV196630:REJ196630 RNR196630:ROF196630 RXN196630:RYB196630 SHJ196630:SHX196630 SRF196630:SRT196630 TBB196630:TBP196630 TKX196630:TLL196630 TUT196630:TVH196630 UEP196630:UFD196630 UOL196630:UOZ196630 UYH196630:UYV196630 VID196630:VIR196630 VRZ196630:VSN196630 WBV196630:WCJ196630 WLR196630:WMF196630 WVN196630:WWB196630 F262166:T262166 JB262166:JP262166 SX262166:TL262166 ACT262166:ADH262166 AMP262166:AND262166 AWL262166:AWZ262166 BGH262166:BGV262166 BQD262166:BQR262166 BZZ262166:CAN262166 CJV262166:CKJ262166 CTR262166:CUF262166 DDN262166:DEB262166 DNJ262166:DNX262166 DXF262166:DXT262166 EHB262166:EHP262166 EQX262166:ERL262166 FAT262166:FBH262166 FKP262166:FLD262166 FUL262166:FUZ262166 GEH262166:GEV262166 GOD262166:GOR262166 GXZ262166:GYN262166 HHV262166:HIJ262166 HRR262166:HSF262166 IBN262166:ICB262166 ILJ262166:ILX262166 IVF262166:IVT262166 JFB262166:JFP262166 JOX262166:JPL262166 JYT262166:JZH262166 KIP262166:KJD262166 KSL262166:KSZ262166 LCH262166:LCV262166 LMD262166:LMR262166 LVZ262166:LWN262166 MFV262166:MGJ262166 MPR262166:MQF262166 MZN262166:NAB262166 NJJ262166:NJX262166 NTF262166:NTT262166 ODB262166:ODP262166 OMX262166:ONL262166 OWT262166:OXH262166 PGP262166:PHD262166 PQL262166:PQZ262166 QAH262166:QAV262166 QKD262166:QKR262166 QTZ262166:QUN262166 RDV262166:REJ262166 RNR262166:ROF262166 RXN262166:RYB262166 SHJ262166:SHX262166 SRF262166:SRT262166 TBB262166:TBP262166 TKX262166:TLL262166 TUT262166:TVH262166 UEP262166:UFD262166 UOL262166:UOZ262166 UYH262166:UYV262166 VID262166:VIR262166 VRZ262166:VSN262166 WBV262166:WCJ262166 WLR262166:WMF262166 WVN262166:WWB262166 F327702:T327702 JB327702:JP327702 SX327702:TL327702 ACT327702:ADH327702 AMP327702:AND327702 AWL327702:AWZ327702 BGH327702:BGV327702 BQD327702:BQR327702 BZZ327702:CAN327702 CJV327702:CKJ327702 CTR327702:CUF327702 DDN327702:DEB327702 DNJ327702:DNX327702 DXF327702:DXT327702 EHB327702:EHP327702 EQX327702:ERL327702 FAT327702:FBH327702 FKP327702:FLD327702 FUL327702:FUZ327702 GEH327702:GEV327702 GOD327702:GOR327702 GXZ327702:GYN327702 HHV327702:HIJ327702 HRR327702:HSF327702 IBN327702:ICB327702 ILJ327702:ILX327702 IVF327702:IVT327702 JFB327702:JFP327702 JOX327702:JPL327702 JYT327702:JZH327702 KIP327702:KJD327702 KSL327702:KSZ327702 LCH327702:LCV327702 LMD327702:LMR327702 LVZ327702:LWN327702 MFV327702:MGJ327702 MPR327702:MQF327702 MZN327702:NAB327702 NJJ327702:NJX327702 NTF327702:NTT327702 ODB327702:ODP327702 OMX327702:ONL327702 OWT327702:OXH327702 PGP327702:PHD327702 PQL327702:PQZ327702 QAH327702:QAV327702 QKD327702:QKR327702 QTZ327702:QUN327702 RDV327702:REJ327702 RNR327702:ROF327702 RXN327702:RYB327702 SHJ327702:SHX327702 SRF327702:SRT327702 TBB327702:TBP327702 TKX327702:TLL327702 TUT327702:TVH327702 UEP327702:UFD327702 UOL327702:UOZ327702 UYH327702:UYV327702 VID327702:VIR327702 VRZ327702:VSN327702 WBV327702:WCJ327702 WLR327702:WMF327702 WVN327702:WWB327702 F393238:T393238 JB393238:JP393238 SX393238:TL393238 ACT393238:ADH393238 AMP393238:AND393238 AWL393238:AWZ393238 BGH393238:BGV393238 BQD393238:BQR393238 BZZ393238:CAN393238 CJV393238:CKJ393238 CTR393238:CUF393238 DDN393238:DEB393238 DNJ393238:DNX393238 DXF393238:DXT393238 EHB393238:EHP393238 EQX393238:ERL393238 FAT393238:FBH393238 FKP393238:FLD393238 FUL393238:FUZ393238 GEH393238:GEV393238 GOD393238:GOR393238 GXZ393238:GYN393238 HHV393238:HIJ393238 HRR393238:HSF393238 IBN393238:ICB393238 ILJ393238:ILX393238 IVF393238:IVT393238 JFB393238:JFP393238 JOX393238:JPL393238 JYT393238:JZH393238 KIP393238:KJD393238 KSL393238:KSZ393238 LCH393238:LCV393238 LMD393238:LMR393238 LVZ393238:LWN393238 MFV393238:MGJ393238 MPR393238:MQF393238 MZN393238:NAB393238 NJJ393238:NJX393238 NTF393238:NTT393238 ODB393238:ODP393238 OMX393238:ONL393238 OWT393238:OXH393238 PGP393238:PHD393238 PQL393238:PQZ393238 QAH393238:QAV393238 QKD393238:QKR393238 QTZ393238:QUN393238 RDV393238:REJ393238 RNR393238:ROF393238 RXN393238:RYB393238 SHJ393238:SHX393238 SRF393238:SRT393238 TBB393238:TBP393238 TKX393238:TLL393238 TUT393238:TVH393238 UEP393238:UFD393238 UOL393238:UOZ393238 UYH393238:UYV393238 VID393238:VIR393238 VRZ393238:VSN393238 WBV393238:WCJ393238 WLR393238:WMF393238 WVN393238:WWB393238 F458774:T458774 JB458774:JP458774 SX458774:TL458774 ACT458774:ADH458774 AMP458774:AND458774 AWL458774:AWZ458774 BGH458774:BGV458774 BQD458774:BQR458774 BZZ458774:CAN458774 CJV458774:CKJ458774 CTR458774:CUF458774 DDN458774:DEB458774 DNJ458774:DNX458774 DXF458774:DXT458774 EHB458774:EHP458774 EQX458774:ERL458774 FAT458774:FBH458774 FKP458774:FLD458774 FUL458774:FUZ458774 GEH458774:GEV458774 GOD458774:GOR458774 GXZ458774:GYN458774 HHV458774:HIJ458774 HRR458774:HSF458774 IBN458774:ICB458774 ILJ458774:ILX458774 IVF458774:IVT458774 JFB458774:JFP458774 JOX458774:JPL458774 JYT458774:JZH458774 KIP458774:KJD458774 KSL458774:KSZ458774 LCH458774:LCV458774 LMD458774:LMR458774 LVZ458774:LWN458774 MFV458774:MGJ458774 MPR458774:MQF458774 MZN458774:NAB458774 NJJ458774:NJX458774 NTF458774:NTT458774 ODB458774:ODP458774 OMX458774:ONL458774 OWT458774:OXH458774 PGP458774:PHD458774 PQL458774:PQZ458774 QAH458774:QAV458774 QKD458774:QKR458774 QTZ458774:QUN458774 RDV458774:REJ458774 RNR458774:ROF458774 RXN458774:RYB458774 SHJ458774:SHX458774 SRF458774:SRT458774 TBB458774:TBP458774 TKX458774:TLL458774 TUT458774:TVH458774 UEP458774:UFD458774 UOL458774:UOZ458774 UYH458774:UYV458774 VID458774:VIR458774 VRZ458774:VSN458774 WBV458774:WCJ458774 WLR458774:WMF458774 WVN458774:WWB458774 F524310:T524310 JB524310:JP524310 SX524310:TL524310 ACT524310:ADH524310 AMP524310:AND524310 AWL524310:AWZ524310 BGH524310:BGV524310 BQD524310:BQR524310 BZZ524310:CAN524310 CJV524310:CKJ524310 CTR524310:CUF524310 DDN524310:DEB524310 DNJ524310:DNX524310 DXF524310:DXT524310 EHB524310:EHP524310 EQX524310:ERL524310 FAT524310:FBH524310 FKP524310:FLD524310 FUL524310:FUZ524310 GEH524310:GEV524310 GOD524310:GOR524310 GXZ524310:GYN524310 HHV524310:HIJ524310 HRR524310:HSF524310 IBN524310:ICB524310 ILJ524310:ILX524310 IVF524310:IVT524310 JFB524310:JFP524310 JOX524310:JPL524310 JYT524310:JZH524310 KIP524310:KJD524310 KSL524310:KSZ524310 LCH524310:LCV524310 LMD524310:LMR524310 LVZ524310:LWN524310 MFV524310:MGJ524310 MPR524310:MQF524310 MZN524310:NAB524310 NJJ524310:NJX524310 NTF524310:NTT524310 ODB524310:ODP524310 OMX524310:ONL524310 OWT524310:OXH524310 PGP524310:PHD524310 PQL524310:PQZ524310 QAH524310:QAV524310 QKD524310:QKR524310 QTZ524310:QUN524310 RDV524310:REJ524310 RNR524310:ROF524310 RXN524310:RYB524310 SHJ524310:SHX524310 SRF524310:SRT524310 TBB524310:TBP524310 TKX524310:TLL524310 TUT524310:TVH524310 UEP524310:UFD524310 UOL524310:UOZ524310 UYH524310:UYV524310 VID524310:VIR524310 VRZ524310:VSN524310 WBV524310:WCJ524310 WLR524310:WMF524310 WVN524310:WWB524310 F589846:T589846 JB589846:JP589846 SX589846:TL589846 ACT589846:ADH589846 AMP589846:AND589846 AWL589846:AWZ589846 BGH589846:BGV589846 BQD589846:BQR589846 BZZ589846:CAN589846 CJV589846:CKJ589846 CTR589846:CUF589846 DDN589846:DEB589846 DNJ589846:DNX589846 DXF589846:DXT589846 EHB589846:EHP589846 EQX589846:ERL589846 FAT589846:FBH589846 FKP589846:FLD589846 FUL589846:FUZ589846 GEH589846:GEV589846 GOD589846:GOR589846 GXZ589846:GYN589846 HHV589846:HIJ589846 HRR589846:HSF589846 IBN589846:ICB589846 ILJ589846:ILX589846 IVF589846:IVT589846 JFB589846:JFP589846 JOX589846:JPL589846 JYT589846:JZH589846 KIP589846:KJD589846 KSL589846:KSZ589846 LCH589846:LCV589846 LMD589846:LMR589846 LVZ589846:LWN589846 MFV589846:MGJ589846 MPR589846:MQF589846 MZN589846:NAB589846 NJJ589846:NJX589846 NTF589846:NTT589846 ODB589846:ODP589846 OMX589846:ONL589846 OWT589846:OXH589846 PGP589846:PHD589846 PQL589846:PQZ589846 QAH589846:QAV589846 QKD589846:QKR589846 QTZ589846:QUN589846 RDV589846:REJ589846 RNR589846:ROF589846 RXN589846:RYB589846 SHJ589846:SHX589846 SRF589846:SRT589846 TBB589846:TBP589846 TKX589846:TLL589846 TUT589846:TVH589846 UEP589846:UFD589846 UOL589846:UOZ589846 UYH589846:UYV589846 VID589846:VIR589846 VRZ589846:VSN589846 WBV589846:WCJ589846 WLR589846:WMF589846 WVN589846:WWB589846 F655382:T655382 JB655382:JP655382 SX655382:TL655382 ACT655382:ADH655382 AMP655382:AND655382 AWL655382:AWZ655382 BGH655382:BGV655382 BQD655382:BQR655382 BZZ655382:CAN655382 CJV655382:CKJ655382 CTR655382:CUF655382 DDN655382:DEB655382 DNJ655382:DNX655382 DXF655382:DXT655382 EHB655382:EHP655382 EQX655382:ERL655382 FAT655382:FBH655382 FKP655382:FLD655382 FUL655382:FUZ655382 GEH655382:GEV655382 GOD655382:GOR655382 GXZ655382:GYN655382 HHV655382:HIJ655382 HRR655382:HSF655382 IBN655382:ICB655382 ILJ655382:ILX655382 IVF655382:IVT655382 JFB655382:JFP655382 JOX655382:JPL655382 JYT655382:JZH655382 KIP655382:KJD655382 KSL655382:KSZ655382 LCH655382:LCV655382 LMD655382:LMR655382 LVZ655382:LWN655382 MFV655382:MGJ655382 MPR655382:MQF655382 MZN655382:NAB655382 NJJ655382:NJX655382 NTF655382:NTT655382 ODB655382:ODP655382 OMX655382:ONL655382 OWT655382:OXH655382 PGP655382:PHD655382 PQL655382:PQZ655382 QAH655382:QAV655382 QKD655382:QKR655382 QTZ655382:QUN655382 RDV655382:REJ655382 RNR655382:ROF655382 RXN655382:RYB655382 SHJ655382:SHX655382 SRF655382:SRT655382 TBB655382:TBP655382 TKX655382:TLL655382 TUT655382:TVH655382 UEP655382:UFD655382 UOL655382:UOZ655382 UYH655382:UYV655382 VID655382:VIR655382 VRZ655382:VSN655382 WBV655382:WCJ655382 WLR655382:WMF655382 WVN655382:WWB655382 F720918:T720918 JB720918:JP720918 SX720918:TL720918 ACT720918:ADH720918 AMP720918:AND720918 AWL720918:AWZ720918 BGH720918:BGV720918 BQD720918:BQR720918 BZZ720918:CAN720918 CJV720918:CKJ720918 CTR720918:CUF720918 DDN720918:DEB720918 DNJ720918:DNX720918 DXF720918:DXT720918 EHB720918:EHP720918 EQX720918:ERL720918 FAT720918:FBH720918 FKP720918:FLD720918 FUL720918:FUZ720918 GEH720918:GEV720918 GOD720918:GOR720918 GXZ720918:GYN720918 HHV720918:HIJ720918 HRR720918:HSF720918 IBN720918:ICB720918 ILJ720918:ILX720918 IVF720918:IVT720918 JFB720918:JFP720918 JOX720918:JPL720918 JYT720918:JZH720918 KIP720918:KJD720918 KSL720918:KSZ720918 LCH720918:LCV720918 LMD720918:LMR720918 LVZ720918:LWN720918 MFV720918:MGJ720918 MPR720918:MQF720918 MZN720918:NAB720918 NJJ720918:NJX720918 NTF720918:NTT720918 ODB720918:ODP720918 OMX720918:ONL720918 OWT720918:OXH720918 PGP720918:PHD720918 PQL720918:PQZ720918 QAH720918:QAV720918 QKD720918:QKR720918 QTZ720918:QUN720918 RDV720918:REJ720918 RNR720918:ROF720918 RXN720918:RYB720918 SHJ720918:SHX720918 SRF720918:SRT720918 TBB720918:TBP720918 TKX720918:TLL720918 TUT720918:TVH720918 UEP720918:UFD720918 UOL720918:UOZ720918 UYH720918:UYV720918 VID720918:VIR720918 VRZ720918:VSN720918 WBV720918:WCJ720918 WLR720918:WMF720918 WVN720918:WWB720918 F786454:T786454 JB786454:JP786454 SX786454:TL786454 ACT786454:ADH786454 AMP786454:AND786454 AWL786454:AWZ786454 BGH786454:BGV786454 BQD786454:BQR786454 BZZ786454:CAN786454 CJV786454:CKJ786454 CTR786454:CUF786454 DDN786454:DEB786454 DNJ786454:DNX786454 DXF786454:DXT786454 EHB786454:EHP786454 EQX786454:ERL786454 FAT786454:FBH786454 FKP786454:FLD786454 FUL786454:FUZ786454 GEH786454:GEV786454 GOD786454:GOR786454 GXZ786454:GYN786454 HHV786454:HIJ786454 HRR786454:HSF786454 IBN786454:ICB786454 ILJ786454:ILX786454 IVF786454:IVT786454 JFB786454:JFP786454 JOX786454:JPL786454 JYT786454:JZH786454 KIP786454:KJD786454 KSL786454:KSZ786454 LCH786454:LCV786454 LMD786454:LMR786454 LVZ786454:LWN786454 MFV786454:MGJ786454 MPR786454:MQF786454 MZN786454:NAB786454 NJJ786454:NJX786454 NTF786454:NTT786454 ODB786454:ODP786454 OMX786454:ONL786454 OWT786454:OXH786454 PGP786454:PHD786454 PQL786454:PQZ786454 QAH786454:QAV786454 QKD786454:QKR786454 QTZ786454:QUN786454 RDV786454:REJ786454 RNR786454:ROF786454 RXN786454:RYB786454 SHJ786454:SHX786454 SRF786454:SRT786454 TBB786454:TBP786454 TKX786454:TLL786454 TUT786454:TVH786454 UEP786454:UFD786454 UOL786454:UOZ786454 UYH786454:UYV786454 VID786454:VIR786454 VRZ786454:VSN786454 WBV786454:WCJ786454 WLR786454:WMF786454 WVN786454:WWB786454 F851990:T851990 JB851990:JP851990 SX851990:TL851990 ACT851990:ADH851990 AMP851990:AND851990 AWL851990:AWZ851990 BGH851990:BGV851990 BQD851990:BQR851990 BZZ851990:CAN851990 CJV851990:CKJ851990 CTR851990:CUF851990 DDN851990:DEB851990 DNJ851990:DNX851990 DXF851990:DXT851990 EHB851990:EHP851990 EQX851990:ERL851990 FAT851990:FBH851990 FKP851990:FLD851990 FUL851990:FUZ851990 GEH851990:GEV851990 GOD851990:GOR851990 GXZ851990:GYN851990 HHV851990:HIJ851990 HRR851990:HSF851990 IBN851990:ICB851990 ILJ851990:ILX851990 IVF851990:IVT851990 JFB851990:JFP851990 JOX851990:JPL851990 JYT851990:JZH851990 KIP851990:KJD851990 KSL851990:KSZ851990 LCH851990:LCV851990 LMD851990:LMR851990 LVZ851990:LWN851990 MFV851990:MGJ851990 MPR851990:MQF851990 MZN851990:NAB851990 NJJ851990:NJX851990 NTF851990:NTT851990 ODB851990:ODP851990 OMX851990:ONL851990 OWT851990:OXH851990 PGP851990:PHD851990 PQL851990:PQZ851990 QAH851990:QAV851990 QKD851990:QKR851990 QTZ851990:QUN851990 RDV851990:REJ851990 RNR851990:ROF851990 RXN851990:RYB851990 SHJ851990:SHX851990 SRF851990:SRT851990 TBB851990:TBP851990 TKX851990:TLL851990 TUT851990:TVH851990 UEP851990:UFD851990 UOL851990:UOZ851990 UYH851990:UYV851990 VID851990:VIR851990 VRZ851990:VSN851990 WBV851990:WCJ851990 WLR851990:WMF851990 WVN851990:WWB851990 F917526:T917526 JB917526:JP917526 SX917526:TL917526 ACT917526:ADH917526 AMP917526:AND917526 AWL917526:AWZ917526 BGH917526:BGV917526 BQD917526:BQR917526 BZZ917526:CAN917526 CJV917526:CKJ917526 CTR917526:CUF917526 DDN917526:DEB917526 DNJ917526:DNX917526 DXF917526:DXT917526 EHB917526:EHP917526 EQX917526:ERL917526 FAT917526:FBH917526 FKP917526:FLD917526 FUL917526:FUZ917526 GEH917526:GEV917526 GOD917526:GOR917526 GXZ917526:GYN917526 HHV917526:HIJ917526 HRR917526:HSF917526 IBN917526:ICB917526 ILJ917526:ILX917526 IVF917526:IVT917526 JFB917526:JFP917526 JOX917526:JPL917526 JYT917526:JZH917526 KIP917526:KJD917526 KSL917526:KSZ917526 LCH917526:LCV917526 LMD917526:LMR917526 LVZ917526:LWN917526 MFV917526:MGJ917526 MPR917526:MQF917526 MZN917526:NAB917526 NJJ917526:NJX917526 NTF917526:NTT917526 ODB917526:ODP917526 OMX917526:ONL917526 OWT917526:OXH917526 PGP917526:PHD917526 PQL917526:PQZ917526 QAH917526:QAV917526 QKD917526:QKR917526 QTZ917526:QUN917526 RDV917526:REJ917526 RNR917526:ROF917526 RXN917526:RYB917526 SHJ917526:SHX917526 SRF917526:SRT917526 TBB917526:TBP917526 TKX917526:TLL917526 TUT917526:TVH917526 UEP917526:UFD917526 UOL917526:UOZ917526 UYH917526:UYV917526 VID917526:VIR917526 VRZ917526:VSN917526 WBV917526:WCJ917526 WLR917526:WMF917526 WVN917526:WWB917526 F983062:T983062 JB983062:JP983062 SX983062:TL983062 ACT983062:ADH983062 AMP983062:AND983062 AWL983062:AWZ983062 BGH983062:BGV983062 BQD983062:BQR983062 BZZ983062:CAN983062 CJV983062:CKJ983062 CTR983062:CUF983062 DDN983062:DEB983062 DNJ983062:DNX983062 DXF983062:DXT983062 EHB983062:EHP983062 EQX983062:ERL983062 FAT983062:FBH983062 FKP983062:FLD983062 FUL983062:FUZ983062 GEH983062:GEV983062 GOD983062:GOR983062 GXZ983062:GYN983062 HHV983062:HIJ983062 HRR983062:HSF983062 IBN983062:ICB983062 ILJ983062:ILX983062 IVF983062:IVT983062 JFB983062:JFP983062 JOX983062:JPL983062 JYT983062:JZH983062 KIP983062:KJD983062 KSL983062:KSZ983062 LCH983062:LCV983062 LMD983062:LMR983062 LVZ983062:LWN983062 MFV983062:MGJ983062 MPR983062:MQF983062 MZN983062:NAB983062 NJJ983062:NJX983062 NTF983062:NTT983062 ODB983062:ODP983062 OMX983062:ONL983062 OWT983062:OXH983062 PGP983062:PHD983062 PQL983062:PQZ983062 QAH983062:QAV983062 QKD983062:QKR983062 QTZ983062:QUN983062 RDV983062:REJ983062 RNR983062:ROF983062 RXN983062:RYB983062 SHJ983062:SHX983062 SRF983062:SRT983062 TBB983062:TBP983062 TKX983062:TLL983062 TUT983062:TVH983062 UEP983062:UFD983062 UOL983062:UOZ983062 UYH983062:UYV983062 VID983062:VIR983062 VRZ983062:VSN983062 WBV983062:WCJ983062 WLR983062:WMF983062 WVN983062:WWB983062">
@@ -6636,7 +6636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -7097,51 +7097,51 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:26">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="93"/>
-      <c r="F2" s="94" t="s">
+      <c r="B2" s="64"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="66"/>
+      <c r="F2" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="96"/>
-      <c r="N2" s="96"/>
-      <c r="O2" s="96"/>
-      <c r="P2" s="96"/>
-      <c r="Q2" s="96"/>
-      <c r="R2" s="96"/>
-      <c r="S2" s="96"/>
-      <c r="T2" s="97"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="69"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="69"/>
+      <c r="T2" s="70"/>
     </row>
     <row r="3" spans="1:26">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="98" t="s">
+      <c r="B3" s="72"/>
+      <c r="C3" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="99"/>
-      <c r="E3" s="100"/>
-      <c r="F3" s="82" t="s">
+      <c r="D3" s="74"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="87"/>
-      <c r="M3" s="88"/>
-      <c r="N3" s="88"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="79"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
@@ -7150,112 +7150,112 @@
       <c r="T3" s="6"/>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="79"/>
+      <c r="B4" s="72"/>
       <c r="C4" s="80"/>
       <c r="D4" s="81"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="82" t="s">
+      <c r="F4" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="84"/>
-      <c r="M4" s="85"/>
-      <c r="N4" s="85"/>
-      <c r="O4" s="85"/>
-      <c r="P4" s="85"/>
-      <c r="Q4" s="85"/>
-      <c r="R4" s="85"/>
-      <c r="S4" s="85"/>
-      <c r="T4" s="86"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="83"/>
+      <c r="N4" s="83"/>
+      <c r="O4" s="83"/>
+      <c r="P4" s="83"/>
+      <c r="Q4" s="83"/>
+      <c r="R4" s="83"/>
+      <c r="S4" s="83"/>
+      <c r="T4" s="84"/>
       <c r="V4" s="8"/>
     </row>
     <row r="5" spans="1:26">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="79"/>
-      <c r="C5" s="87" t="s">
+      <c r="B5" s="72"/>
+      <c r="C5" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="88"/>
-      <c r="K5" s="88"/>
-      <c r="L5" s="88"/>
-      <c r="M5" s="88"/>
-      <c r="N5" s="88"/>
-      <c r="O5" s="88"/>
-      <c r="P5" s="88"/>
-      <c r="Q5" s="88"/>
-      <c r="R5" s="88"/>
-      <c r="S5" s="88"/>
-      <c r="T5" s="89"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="79"/>
+      <c r="N5" s="79"/>
+      <c r="O5" s="79"/>
+      <c r="P5" s="79"/>
+      <c r="Q5" s="79"/>
+      <c r="R5" s="79"/>
+      <c r="S5" s="79"/>
+      <c r="T5" s="85"/>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="68"/>
-      <c r="C6" s="69" t="s">
+      <c r="B6" s="100"/>
+      <c r="C6" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="70"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="69" t="s">
+      <c r="D6" s="87"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="69" t="s">
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="87"/>
+      <c r="K6" s="88"/>
+      <c r="L6" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="70"/>
-      <c r="N6" s="71"/>
-      <c r="O6" s="69" t="s">
+      <c r="M6" s="87"/>
+      <c r="N6" s="88"/>
+      <c r="O6" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="70"/>
-      <c r="Q6" s="70"/>
-      <c r="R6" s="70"/>
-      <c r="S6" s="70"/>
-      <c r="T6" s="72"/>
+      <c r="P6" s="87"/>
+      <c r="Q6" s="87"/>
+      <c r="R6" s="87"/>
+      <c r="S6" s="87"/>
+      <c r="T6" s="89"/>
       <c r="V6" s="8"/>
     </row>
     <row r="7" spans="1:26" ht="11.25" thickBot="1">
-      <c r="A7" s="73">
+      <c r="A7" s="90">
         <f>COUNTIF(F23:HQ23,"P")</f>
         <v>3</v>
       </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="75">
+      <c r="B7" s="91"/>
+      <c r="C7" s="92">
         <f>COUNTIF(F23:HQ23,"F")</f>
         <v>0</v>
       </c>
-      <c r="D7" s="76"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="75">
+      <c r="D7" s="93"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="92">
         <f>SUM(O7,-A7,-C7)</f>
         <v>18</v>
       </c>
-      <c r="G7" s="76"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="76"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="74"/>
+      <c r="G7" s="93"/>
+      <c r="H7" s="93"/>
+      <c r="I7" s="93"/>
+      <c r="J7" s="93"/>
+      <c r="K7" s="91"/>
       <c r="L7" s="9">
         <f>COUNTIF(E22:HQ22,"N")</f>
         <v>0</v>
@@ -7268,15 +7268,15 @@
         <f>COUNTIF(E22:HQ22,"B")</f>
         <v>0</v>
       </c>
-      <c r="O7" s="75">
+      <c r="O7" s="92">
         <f>COUNTA(E9:HT9)</f>
         <v>21</v>
       </c>
-      <c r="P7" s="76"/>
-      <c r="Q7" s="76"/>
-      <c r="R7" s="76"/>
-      <c r="S7" s="76"/>
-      <c r="T7" s="77"/>
+      <c r="P7" s="93"/>
+      <c r="Q7" s="93"/>
+      <c r="R7" s="93"/>
+      <c r="S7" s="93"/>
+      <c r="T7" s="94"/>
       <c r="U7" s="10"/>
     </row>
     <row r="8" spans="1:26" ht="11.25" thickBot="1"/>
@@ -7359,7 +7359,7 @@
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" s="22"/>
       <c r="F10" s="23" t="s">
@@ -7391,7 +7391,7 @@
       <c r="B11" s="19"/>
       <c r="C11" s="20"/>
       <c r="D11" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" s="26"/>
       <c r="F11" s="23"/>
@@ -7423,7 +7423,7 @@
       <c r="B12" s="19"/>
       <c r="C12" s="20"/>
       <c r="D12" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" s="26"/>
       <c r="F12" s="23"/>
@@ -7724,11 +7724,11 @@
       <c r="A22" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="63" t="s">
+      <c r="B22" s="95" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="95"/>
       <c r="E22" s="49"/>
       <c r="F22" s="50"/>
       <c r="G22" s="50"/>
@@ -7754,11 +7754,11 @@
     </row>
     <row r="23" spans="1:26" ht="11.25">
       <c r="A23" s="52"/>
-      <c r="B23" s="64" t="s">
+      <c r="B23" s="96" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="96"/>
       <c r="E23" s="53"/>
       <c r="F23" s="54" t="s">
         <v>46</v>
@@ -7790,11 +7790,11 @@
     </row>
     <row r="24" spans="1:26">
       <c r="A24" s="52"/>
-      <c r="B24" s="65" t="s">
+      <c r="B24" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
+      <c r="C24" s="97"/>
+      <c r="D24" s="97"/>
       <c r="E24" s="56"/>
       <c r="F24" s="57"/>
       <c r="G24" s="57"/>
@@ -7820,11 +7820,11 @@
     </row>
     <row r="25" spans="1:26" ht="11.25" thickBot="1">
       <c r="A25" s="59"/>
-      <c r="B25" s="66" t="s">
+      <c r="B25" s="98" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="66"/>
-      <c r="D25" s="66"/>
+      <c r="C25" s="98"/>
+      <c r="D25" s="98"/>
       <c r="E25" s="60"/>
       <c r="F25" s="61"/>
       <c r="G25" s="61"/>
@@ -7856,6 +7856,25 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="F6:K6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="O6:T6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="F7:K7"/>
+    <mergeCell ref="O7:T7"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="L4:T4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:T5"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:K2"/>
@@ -7864,25 +7883,6 @@
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="F3:K3"/>
     <mergeCell ref="L3:N3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:K4"/>
-    <mergeCell ref="L4:T4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:T5"/>
-    <mergeCell ref="F6:K6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="O6:T6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="F7:K7"/>
-    <mergeCell ref="O7:T7"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:E6"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F22:T22 JB22:JP22 SX22:TL22 ACT22:ADH22 AMP22:AND22 AWL22:AWZ22 BGH22:BGV22 BQD22:BQR22 BZZ22:CAN22 CJV22:CKJ22 CTR22:CUF22 DDN22:DEB22 DNJ22:DNX22 DXF22:DXT22 EHB22:EHP22 EQX22:ERL22 FAT22:FBH22 FKP22:FLD22 FUL22:FUZ22 GEH22:GEV22 GOD22:GOR22 GXZ22:GYN22 HHV22:HIJ22 HRR22:HSF22 IBN22:ICB22 ILJ22:ILX22 IVF22:IVT22 JFB22:JFP22 JOX22:JPL22 JYT22:JZH22 KIP22:KJD22 KSL22:KSZ22 LCH22:LCV22 LMD22:LMR22 LVZ22:LWN22 MFV22:MGJ22 MPR22:MQF22 MZN22:NAB22 NJJ22:NJX22 NTF22:NTT22 ODB22:ODP22 OMX22:ONL22 OWT22:OXH22 PGP22:PHD22 PQL22:PQZ22 QAH22:QAV22 QKD22:QKR22 QTZ22:QUN22 RDV22:REJ22 RNR22:ROF22 RXN22:RYB22 SHJ22:SHX22 SRF22:SRT22 TBB22:TBP22 TKX22:TLL22 TUT22:TVH22 UEP22:UFD22 UOL22:UOZ22 UYH22:UYV22 VID22:VIR22 VRZ22:VSN22 WBV22:WCJ22 WLR22:WMF22 WVN22:WWB22 F65558:T65558 JB65558:JP65558 SX65558:TL65558 ACT65558:ADH65558 AMP65558:AND65558 AWL65558:AWZ65558 BGH65558:BGV65558 BQD65558:BQR65558 BZZ65558:CAN65558 CJV65558:CKJ65558 CTR65558:CUF65558 DDN65558:DEB65558 DNJ65558:DNX65558 DXF65558:DXT65558 EHB65558:EHP65558 EQX65558:ERL65558 FAT65558:FBH65558 FKP65558:FLD65558 FUL65558:FUZ65558 GEH65558:GEV65558 GOD65558:GOR65558 GXZ65558:GYN65558 HHV65558:HIJ65558 HRR65558:HSF65558 IBN65558:ICB65558 ILJ65558:ILX65558 IVF65558:IVT65558 JFB65558:JFP65558 JOX65558:JPL65558 JYT65558:JZH65558 KIP65558:KJD65558 KSL65558:KSZ65558 LCH65558:LCV65558 LMD65558:LMR65558 LVZ65558:LWN65558 MFV65558:MGJ65558 MPR65558:MQF65558 MZN65558:NAB65558 NJJ65558:NJX65558 NTF65558:NTT65558 ODB65558:ODP65558 OMX65558:ONL65558 OWT65558:OXH65558 PGP65558:PHD65558 PQL65558:PQZ65558 QAH65558:QAV65558 QKD65558:QKR65558 QTZ65558:QUN65558 RDV65558:REJ65558 RNR65558:ROF65558 RXN65558:RYB65558 SHJ65558:SHX65558 SRF65558:SRT65558 TBB65558:TBP65558 TKX65558:TLL65558 TUT65558:TVH65558 UEP65558:UFD65558 UOL65558:UOZ65558 UYH65558:UYV65558 VID65558:VIR65558 VRZ65558:VSN65558 WBV65558:WCJ65558 WLR65558:WMF65558 WVN65558:WWB65558 F131094:T131094 JB131094:JP131094 SX131094:TL131094 ACT131094:ADH131094 AMP131094:AND131094 AWL131094:AWZ131094 BGH131094:BGV131094 BQD131094:BQR131094 BZZ131094:CAN131094 CJV131094:CKJ131094 CTR131094:CUF131094 DDN131094:DEB131094 DNJ131094:DNX131094 DXF131094:DXT131094 EHB131094:EHP131094 EQX131094:ERL131094 FAT131094:FBH131094 FKP131094:FLD131094 FUL131094:FUZ131094 GEH131094:GEV131094 GOD131094:GOR131094 GXZ131094:GYN131094 HHV131094:HIJ131094 HRR131094:HSF131094 IBN131094:ICB131094 ILJ131094:ILX131094 IVF131094:IVT131094 JFB131094:JFP131094 JOX131094:JPL131094 JYT131094:JZH131094 KIP131094:KJD131094 KSL131094:KSZ131094 LCH131094:LCV131094 LMD131094:LMR131094 LVZ131094:LWN131094 MFV131094:MGJ131094 MPR131094:MQF131094 MZN131094:NAB131094 NJJ131094:NJX131094 NTF131094:NTT131094 ODB131094:ODP131094 OMX131094:ONL131094 OWT131094:OXH131094 PGP131094:PHD131094 PQL131094:PQZ131094 QAH131094:QAV131094 QKD131094:QKR131094 QTZ131094:QUN131094 RDV131094:REJ131094 RNR131094:ROF131094 RXN131094:RYB131094 SHJ131094:SHX131094 SRF131094:SRT131094 TBB131094:TBP131094 TKX131094:TLL131094 TUT131094:TVH131094 UEP131094:UFD131094 UOL131094:UOZ131094 UYH131094:UYV131094 VID131094:VIR131094 VRZ131094:VSN131094 WBV131094:WCJ131094 WLR131094:WMF131094 WVN131094:WWB131094 F196630:T196630 JB196630:JP196630 SX196630:TL196630 ACT196630:ADH196630 AMP196630:AND196630 AWL196630:AWZ196630 BGH196630:BGV196630 BQD196630:BQR196630 BZZ196630:CAN196630 CJV196630:CKJ196630 CTR196630:CUF196630 DDN196630:DEB196630 DNJ196630:DNX196630 DXF196630:DXT196630 EHB196630:EHP196630 EQX196630:ERL196630 FAT196630:FBH196630 FKP196630:FLD196630 FUL196630:FUZ196630 GEH196630:GEV196630 GOD196630:GOR196630 GXZ196630:GYN196630 HHV196630:HIJ196630 HRR196630:HSF196630 IBN196630:ICB196630 ILJ196630:ILX196630 IVF196630:IVT196630 JFB196630:JFP196630 JOX196630:JPL196630 JYT196630:JZH196630 KIP196630:KJD196630 KSL196630:KSZ196630 LCH196630:LCV196630 LMD196630:LMR196630 LVZ196630:LWN196630 MFV196630:MGJ196630 MPR196630:MQF196630 MZN196630:NAB196630 NJJ196630:NJX196630 NTF196630:NTT196630 ODB196630:ODP196630 OMX196630:ONL196630 OWT196630:OXH196630 PGP196630:PHD196630 PQL196630:PQZ196630 QAH196630:QAV196630 QKD196630:QKR196630 QTZ196630:QUN196630 RDV196630:REJ196630 RNR196630:ROF196630 RXN196630:RYB196630 SHJ196630:SHX196630 SRF196630:SRT196630 TBB196630:TBP196630 TKX196630:TLL196630 TUT196630:TVH196630 UEP196630:UFD196630 UOL196630:UOZ196630 UYH196630:UYV196630 VID196630:VIR196630 VRZ196630:VSN196630 WBV196630:WCJ196630 WLR196630:WMF196630 WVN196630:WWB196630 F262166:T262166 JB262166:JP262166 SX262166:TL262166 ACT262166:ADH262166 AMP262166:AND262166 AWL262166:AWZ262166 BGH262166:BGV262166 BQD262166:BQR262166 BZZ262166:CAN262166 CJV262166:CKJ262166 CTR262166:CUF262166 DDN262166:DEB262166 DNJ262166:DNX262166 DXF262166:DXT262166 EHB262166:EHP262166 EQX262166:ERL262166 FAT262166:FBH262166 FKP262166:FLD262166 FUL262166:FUZ262166 GEH262166:GEV262166 GOD262166:GOR262166 GXZ262166:GYN262166 HHV262166:HIJ262166 HRR262166:HSF262166 IBN262166:ICB262166 ILJ262166:ILX262166 IVF262166:IVT262166 JFB262166:JFP262166 JOX262166:JPL262166 JYT262166:JZH262166 KIP262166:KJD262166 KSL262166:KSZ262166 LCH262166:LCV262166 LMD262166:LMR262166 LVZ262166:LWN262166 MFV262166:MGJ262166 MPR262166:MQF262166 MZN262166:NAB262166 NJJ262166:NJX262166 NTF262166:NTT262166 ODB262166:ODP262166 OMX262166:ONL262166 OWT262166:OXH262166 PGP262166:PHD262166 PQL262166:PQZ262166 QAH262166:QAV262166 QKD262166:QKR262166 QTZ262166:QUN262166 RDV262166:REJ262166 RNR262166:ROF262166 RXN262166:RYB262166 SHJ262166:SHX262166 SRF262166:SRT262166 TBB262166:TBP262166 TKX262166:TLL262166 TUT262166:TVH262166 UEP262166:UFD262166 UOL262166:UOZ262166 UYH262166:UYV262166 VID262166:VIR262166 VRZ262166:VSN262166 WBV262166:WCJ262166 WLR262166:WMF262166 WVN262166:WWB262166 F327702:T327702 JB327702:JP327702 SX327702:TL327702 ACT327702:ADH327702 AMP327702:AND327702 AWL327702:AWZ327702 BGH327702:BGV327702 BQD327702:BQR327702 BZZ327702:CAN327702 CJV327702:CKJ327702 CTR327702:CUF327702 DDN327702:DEB327702 DNJ327702:DNX327702 DXF327702:DXT327702 EHB327702:EHP327702 EQX327702:ERL327702 FAT327702:FBH327702 FKP327702:FLD327702 FUL327702:FUZ327702 GEH327702:GEV327702 GOD327702:GOR327702 GXZ327702:GYN327702 HHV327702:HIJ327702 HRR327702:HSF327702 IBN327702:ICB327702 ILJ327702:ILX327702 IVF327702:IVT327702 JFB327702:JFP327702 JOX327702:JPL327702 JYT327702:JZH327702 KIP327702:KJD327702 KSL327702:KSZ327702 LCH327702:LCV327702 LMD327702:LMR327702 LVZ327702:LWN327702 MFV327702:MGJ327702 MPR327702:MQF327702 MZN327702:NAB327702 NJJ327702:NJX327702 NTF327702:NTT327702 ODB327702:ODP327702 OMX327702:ONL327702 OWT327702:OXH327702 PGP327702:PHD327702 PQL327702:PQZ327702 QAH327702:QAV327702 QKD327702:QKR327702 QTZ327702:QUN327702 RDV327702:REJ327702 RNR327702:ROF327702 RXN327702:RYB327702 SHJ327702:SHX327702 SRF327702:SRT327702 TBB327702:TBP327702 TKX327702:TLL327702 TUT327702:TVH327702 UEP327702:UFD327702 UOL327702:UOZ327702 UYH327702:UYV327702 VID327702:VIR327702 VRZ327702:VSN327702 WBV327702:WCJ327702 WLR327702:WMF327702 WVN327702:WWB327702 F393238:T393238 JB393238:JP393238 SX393238:TL393238 ACT393238:ADH393238 AMP393238:AND393238 AWL393238:AWZ393238 BGH393238:BGV393238 BQD393238:BQR393238 BZZ393238:CAN393238 CJV393238:CKJ393238 CTR393238:CUF393238 DDN393238:DEB393238 DNJ393238:DNX393238 DXF393238:DXT393238 EHB393238:EHP393238 EQX393238:ERL393238 FAT393238:FBH393238 FKP393238:FLD393238 FUL393238:FUZ393238 GEH393238:GEV393238 GOD393238:GOR393238 GXZ393238:GYN393238 HHV393238:HIJ393238 HRR393238:HSF393238 IBN393238:ICB393238 ILJ393238:ILX393238 IVF393238:IVT393238 JFB393238:JFP393238 JOX393238:JPL393238 JYT393238:JZH393238 KIP393238:KJD393238 KSL393238:KSZ393238 LCH393238:LCV393238 LMD393238:LMR393238 LVZ393238:LWN393238 MFV393238:MGJ393238 MPR393238:MQF393238 MZN393238:NAB393238 NJJ393238:NJX393238 NTF393238:NTT393238 ODB393238:ODP393238 OMX393238:ONL393238 OWT393238:OXH393238 PGP393238:PHD393238 PQL393238:PQZ393238 QAH393238:QAV393238 QKD393238:QKR393238 QTZ393238:QUN393238 RDV393238:REJ393238 RNR393238:ROF393238 RXN393238:RYB393238 SHJ393238:SHX393238 SRF393238:SRT393238 TBB393238:TBP393238 TKX393238:TLL393238 TUT393238:TVH393238 UEP393238:UFD393238 UOL393238:UOZ393238 UYH393238:UYV393238 VID393238:VIR393238 VRZ393238:VSN393238 WBV393238:WCJ393238 WLR393238:WMF393238 WVN393238:WWB393238 F458774:T458774 JB458774:JP458774 SX458774:TL458774 ACT458774:ADH458774 AMP458774:AND458774 AWL458774:AWZ458774 BGH458774:BGV458774 BQD458774:BQR458774 BZZ458774:CAN458774 CJV458774:CKJ458774 CTR458774:CUF458774 DDN458774:DEB458774 DNJ458774:DNX458774 DXF458774:DXT458774 EHB458774:EHP458774 EQX458774:ERL458774 FAT458774:FBH458774 FKP458774:FLD458774 FUL458774:FUZ458774 GEH458774:GEV458774 GOD458774:GOR458774 GXZ458774:GYN458774 HHV458774:HIJ458774 HRR458774:HSF458774 IBN458774:ICB458774 ILJ458774:ILX458774 IVF458774:IVT458774 JFB458774:JFP458774 JOX458774:JPL458774 JYT458774:JZH458774 KIP458774:KJD458774 KSL458774:KSZ458774 LCH458774:LCV458774 LMD458774:LMR458774 LVZ458774:LWN458774 MFV458774:MGJ458774 MPR458774:MQF458774 MZN458774:NAB458774 NJJ458774:NJX458774 NTF458774:NTT458774 ODB458774:ODP458774 OMX458774:ONL458774 OWT458774:OXH458774 PGP458774:PHD458774 PQL458774:PQZ458774 QAH458774:QAV458774 QKD458774:QKR458774 QTZ458774:QUN458774 RDV458774:REJ458774 RNR458774:ROF458774 RXN458774:RYB458774 SHJ458774:SHX458774 SRF458774:SRT458774 TBB458774:TBP458774 TKX458774:TLL458774 TUT458774:TVH458774 UEP458774:UFD458774 UOL458774:UOZ458774 UYH458774:UYV458774 VID458774:VIR458774 VRZ458774:VSN458774 WBV458774:WCJ458774 WLR458774:WMF458774 WVN458774:WWB458774 F524310:T524310 JB524310:JP524310 SX524310:TL524310 ACT524310:ADH524310 AMP524310:AND524310 AWL524310:AWZ524310 BGH524310:BGV524310 BQD524310:BQR524310 BZZ524310:CAN524310 CJV524310:CKJ524310 CTR524310:CUF524310 DDN524310:DEB524310 DNJ524310:DNX524310 DXF524310:DXT524310 EHB524310:EHP524310 EQX524310:ERL524310 FAT524310:FBH524310 FKP524310:FLD524310 FUL524310:FUZ524310 GEH524310:GEV524310 GOD524310:GOR524310 GXZ524310:GYN524310 HHV524310:HIJ524310 HRR524310:HSF524310 IBN524310:ICB524310 ILJ524310:ILX524310 IVF524310:IVT524310 JFB524310:JFP524310 JOX524310:JPL524310 JYT524310:JZH524310 KIP524310:KJD524310 KSL524310:KSZ524310 LCH524310:LCV524310 LMD524310:LMR524310 LVZ524310:LWN524310 MFV524310:MGJ524310 MPR524310:MQF524310 MZN524310:NAB524310 NJJ524310:NJX524310 NTF524310:NTT524310 ODB524310:ODP524310 OMX524310:ONL524310 OWT524310:OXH524310 PGP524310:PHD524310 PQL524310:PQZ524310 QAH524310:QAV524310 QKD524310:QKR524310 QTZ524310:QUN524310 RDV524310:REJ524310 RNR524310:ROF524310 RXN524310:RYB524310 SHJ524310:SHX524310 SRF524310:SRT524310 TBB524310:TBP524310 TKX524310:TLL524310 TUT524310:TVH524310 UEP524310:UFD524310 UOL524310:UOZ524310 UYH524310:UYV524310 VID524310:VIR524310 VRZ524310:VSN524310 WBV524310:WCJ524310 WLR524310:WMF524310 WVN524310:WWB524310 F589846:T589846 JB589846:JP589846 SX589846:TL589846 ACT589846:ADH589846 AMP589846:AND589846 AWL589846:AWZ589846 BGH589846:BGV589846 BQD589846:BQR589846 BZZ589846:CAN589846 CJV589846:CKJ589846 CTR589846:CUF589846 DDN589846:DEB589846 DNJ589846:DNX589846 DXF589846:DXT589846 EHB589846:EHP589846 EQX589846:ERL589846 FAT589846:FBH589846 FKP589846:FLD589846 FUL589846:FUZ589846 GEH589846:GEV589846 GOD589846:GOR589846 GXZ589846:GYN589846 HHV589846:HIJ589846 HRR589846:HSF589846 IBN589846:ICB589846 ILJ589846:ILX589846 IVF589846:IVT589846 JFB589846:JFP589846 JOX589846:JPL589846 JYT589846:JZH589846 KIP589846:KJD589846 KSL589846:KSZ589846 LCH589846:LCV589846 LMD589846:LMR589846 LVZ589846:LWN589846 MFV589846:MGJ589846 MPR589846:MQF589846 MZN589846:NAB589846 NJJ589846:NJX589846 NTF589846:NTT589846 ODB589846:ODP589846 OMX589846:ONL589846 OWT589846:OXH589846 PGP589846:PHD589846 PQL589846:PQZ589846 QAH589846:QAV589846 QKD589846:QKR589846 QTZ589846:QUN589846 RDV589846:REJ589846 RNR589846:ROF589846 RXN589846:RYB589846 SHJ589846:SHX589846 SRF589846:SRT589846 TBB589846:TBP589846 TKX589846:TLL589846 TUT589846:TVH589846 UEP589846:UFD589846 UOL589846:UOZ589846 UYH589846:UYV589846 VID589846:VIR589846 VRZ589846:VSN589846 WBV589846:WCJ589846 WLR589846:WMF589846 WVN589846:WWB589846 F655382:T655382 JB655382:JP655382 SX655382:TL655382 ACT655382:ADH655382 AMP655382:AND655382 AWL655382:AWZ655382 BGH655382:BGV655382 BQD655382:BQR655382 BZZ655382:CAN655382 CJV655382:CKJ655382 CTR655382:CUF655382 DDN655382:DEB655382 DNJ655382:DNX655382 DXF655382:DXT655382 EHB655382:EHP655382 EQX655382:ERL655382 FAT655382:FBH655382 FKP655382:FLD655382 FUL655382:FUZ655382 GEH655382:GEV655382 GOD655382:GOR655382 GXZ655382:GYN655382 HHV655382:HIJ655382 HRR655382:HSF655382 IBN655382:ICB655382 ILJ655382:ILX655382 IVF655382:IVT655382 JFB655382:JFP655382 JOX655382:JPL655382 JYT655382:JZH655382 KIP655382:KJD655382 KSL655382:KSZ655382 LCH655382:LCV655382 LMD655382:LMR655382 LVZ655382:LWN655382 MFV655382:MGJ655382 MPR655382:MQF655382 MZN655382:NAB655382 NJJ655382:NJX655382 NTF655382:NTT655382 ODB655382:ODP655382 OMX655382:ONL655382 OWT655382:OXH655382 PGP655382:PHD655382 PQL655382:PQZ655382 QAH655382:QAV655382 QKD655382:QKR655382 QTZ655382:QUN655382 RDV655382:REJ655382 RNR655382:ROF655382 RXN655382:RYB655382 SHJ655382:SHX655382 SRF655382:SRT655382 TBB655382:TBP655382 TKX655382:TLL655382 TUT655382:TVH655382 UEP655382:UFD655382 UOL655382:UOZ655382 UYH655382:UYV655382 VID655382:VIR655382 VRZ655382:VSN655382 WBV655382:WCJ655382 WLR655382:WMF655382 WVN655382:WWB655382 F720918:T720918 JB720918:JP720918 SX720918:TL720918 ACT720918:ADH720918 AMP720918:AND720918 AWL720918:AWZ720918 BGH720918:BGV720918 BQD720918:BQR720918 BZZ720918:CAN720918 CJV720918:CKJ720918 CTR720918:CUF720918 DDN720918:DEB720918 DNJ720918:DNX720918 DXF720918:DXT720918 EHB720918:EHP720918 EQX720918:ERL720918 FAT720918:FBH720918 FKP720918:FLD720918 FUL720918:FUZ720918 GEH720918:GEV720918 GOD720918:GOR720918 GXZ720918:GYN720918 HHV720918:HIJ720918 HRR720918:HSF720918 IBN720918:ICB720918 ILJ720918:ILX720918 IVF720918:IVT720918 JFB720918:JFP720918 JOX720918:JPL720918 JYT720918:JZH720918 KIP720918:KJD720918 KSL720918:KSZ720918 LCH720918:LCV720918 LMD720918:LMR720918 LVZ720918:LWN720918 MFV720918:MGJ720918 MPR720918:MQF720918 MZN720918:NAB720918 NJJ720918:NJX720918 NTF720918:NTT720918 ODB720918:ODP720918 OMX720918:ONL720918 OWT720918:OXH720918 PGP720918:PHD720918 PQL720918:PQZ720918 QAH720918:QAV720918 QKD720918:QKR720918 QTZ720918:QUN720918 RDV720918:REJ720918 RNR720918:ROF720918 RXN720918:RYB720918 SHJ720918:SHX720918 SRF720918:SRT720918 TBB720918:TBP720918 TKX720918:TLL720918 TUT720918:TVH720918 UEP720918:UFD720918 UOL720918:UOZ720918 UYH720918:UYV720918 VID720918:VIR720918 VRZ720918:VSN720918 WBV720918:WCJ720918 WLR720918:WMF720918 WVN720918:WWB720918 F786454:T786454 JB786454:JP786454 SX786454:TL786454 ACT786454:ADH786454 AMP786454:AND786454 AWL786454:AWZ786454 BGH786454:BGV786454 BQD786454:BQR786454 BZZ786454:CAN786454 CJV786454:CKJ786454 CTR786454:CUF786454 DDN786454:DEB786454 DNJ786454:DNX786454 DXF786454:DXT786454 EHB786454:EHP786454 EQX786454:ERL786454 FAT786454:FBH786454 FKP786454:FLD786454 FUL786454:FUZ786454 GEH786454:GEV786454 GOD786454:GOR786454 GXZ786454:GYN786454 HHV786454:HIJ786454 HRR786454:HSF786454 IBN786454:ICB786454 ILJ786454:ILX786454 IVF786454:IVT786454 JFB786454:JFP786454 JOX786454:JPL786454 JYT786454:JZH786454 KIP786454:KJD786454 KSL786454:KSZ786454 LCH786454:LCV786454 LMD786454:LMR786454 LVZ786454:LWN786454 MFV786454:MGJ786454 MPR786454:MQF786454 MZN786454:NAB786454 NJJ786454:NJX786454 NTF786454:NTT786454 ODB786454:ODP786454 OMX786454:ONL786454 OWT786454:OXH786454 PGP786454:PHD786454 PQL786454:PQZ786454 QAH786454:QAV786454 QKD786454:QKR786454 QTZ786454:QUN786454 RDV786454:REJ786454 RNR786454:ROF786454 RXN786454:RYB786454 SHJ786454:SHX786454 SRF786454:SRT786454 TBB786454:TBP786454 TKX786454:TLL786454 TUT786454:TVH786454 UEP786454:UFD786454 UOL786454:UOZ786454 UYH786454:UYV786454 VID786454:VIR786454 VRZ786454:VSN786454 WBV786454:WCJ786454 WLR786454:WMF786454 WVN786454:WWB786454 F851990:T851990 JB851990:JP851990 SX851990:TL851990 ACT851990:ADH851990 AMP851990:AND851990 AWL851990:AWZ851990 BGH851990:BGV851990 BQD851990:BQR851990 BZZ851990:CAN851990 CJV851990:CKJ851990 CTR851990:CUF851990 DDN851990:DEB851990 DNJ851990:DNX851990 DXF851990:DXT851990 EHB851990:EHP851990 EQX851990:ERL851990 FAT851990:FBH851990 FKP851990:FLD851990 FUL851990:FUZ851990 GEH851990:GEV851990 GOD851990:GOR851990 GXZ851990:GYN851990 HHV851990:HIJ851990 HRR851990:HSF851990 IBN851990:ICB851990 ILJ851990:ILX851990 IVF851990:IVT851990 JFB851990:JFP851990 JOX851990:JPL851990 JYT851990:JZH851990 KIP851990:KJD851990 KSL851990:KSZ851990 LCH851990:LCV851990 LMD851990:LMR851990 LVZ851990:LWN851990 MFV851990:MGJ851990 MPR851990:MQF851990 MZN851990:NAB851990 NJJ851990:NJX851990 NTF851990:NTT851990 ODB851990:ODP851990 OMX851990:ONL851990 OWT851990:OXH851990 PGP851990:PHD851990 PQL851990:PQZ851990 QAH851990:QAV851990 QKD851990:QKR851990 QTZ851990:QUN851990 RDV851990:REJ851990 RNR851990:ROF851990 RXN851990:RYB851990 SHJ851990:SHX851990 SRF851990:SRT851990 TBB851990:TBP851990 TKX851990:TLL851990 TUT851990:TVH851990 UEP851990:UFD851990 UOL851990:UOZ851990 UYH851990:UYV851990 VID851990:VIR851990 VRZ851990:VSN851990 WBV851990:WCJ851990 WLR851990:WMF851990 WVN851990:WWB851990 F917526:T917526 JB917526:JP917526 SX917526:TL917526 ACT917526:ADH917526 AMP917526:AND917526 AWL917526:AWZ917526 BGH917526:BGV917526 BQD917526:BQR917526 BZZ917526:CAN917526 CJV917526:CKJ917526 CTR917526:CUF917526 DDN917526:DEB917526 DNJ917526:DNX917526 DXF917526:DXT917526 EHB917526:EHP917526 EQX917526:ERL917526 FAT917526:FBH917526 FKP917526:FLD917526 FUL917526:FUZ917526 GEH917526:GEV917526 GOD917526:GOR917526 GXZ917526:GYN917526 HHV917526:HIJ917526 HRR917526:HSF917526 IBN917526:ICB917526 ILJ917526:ILX917526 IVF917526:IVT917526 JFB917526:JFP917526 JOX917526:JPL917526 JYT917526:JZH917526 KIP917526:KJD917526 KSL917526:KSZ917526 LCH917526:LCV917526 LMD917526:LMR917526 LVZ917526:LWN917526 MFV917526:MGJ917526 MPR917526:MQF917526 MZN917526:NAB917526 NJJ917526:NJX917526 NTF917526:NTT917526 ODB917526:ODP917526 OMX917526:ONL917526 OWT917526:OXH917526 PGP917526:PHD917526 PQL917526:PQZ917526 QAH917526:QAV917526 QKD917526:QKR917526 QTZ917526:QUN917526 RDV917526:REJ917526 RNR917526:ROF917526 RXN917526:RYB917526 SHJ917526:SHX917526 SRF917526:SRT917526 TBB917526:TBP917526 TKX917526:TLL917526 TUT917526:TVH917526 UEP917526:UFD917526 UOL917526:UOZ917526 UYH917526:UYV917526 VID917526:VIR917526 VRZ917526:VSN917526 WBV917526:WCJ917526 WLR917526:WMF917526 WVN917526:WWB917526 F983062:T983062 JB983062:JP983062 SX983062:TL983062 ACT983062:ADH983062 AMP983062:AND983062 AWL983062:AWZ983062 BGH983062:BGV983062 BQD983062:BQR983062 BZZ983062:CAN983062 CJV983062:CKJ983062 CTR983062:CUF983062 DDN983062:DEB983062 DNJ983062:DNX983062 DXF983062:DXT983062 EHB983062:EHP983062 EQX983062:ERL983062 FAT983062:FBH983062 FKP983062:FLD983062 FUL983062:FUZ983062 GEH983062:GEV983062 GOD983062:GOR983062 GXZ983062:GYN983062 HHV983062:HIJ983062 HRR983062:HSF983062 IBN983062:ICB983062 ILJ983062:ILX983062 IVF983062:IVT983062 JFB983062:JFP983062 JOX983062:JPL983062 JYT983062:JZH983062 KIP983062:KJD983062 KSL983062:KSZ983062 LCH983062:LCV983062 LMD983062:LMR983062 LVZ983062:LWN983062 MFV983062:MGJ983062 MPR983062:MQF983062 MZN983062:NAB983062 NJJ983062:NJX983062 NTF983062:NTT983062 ODB983062:ODP983062 OMX983062:ONL983062 OWT983062:OXH983062 PGP983062:PHD983062 PQL983062:PQZ983062 QAH983062:QAV983062 QKD983062:QKR983062 QTZ983062:QUN983062 RDV983062:REJ983062 RNR983062:ROF983062 RXN983062:RYB983062 SHJ983062:SHX983062 SRF983062:SRT983062 TBB983062:TBP983062 TKX983062:TLL983062 TUT983062:TVH983062 UEP983062:UFD983062 UOL983062:UOZ983062 UYH983062:UYV983062 VID983062:VIR983062 VRZ983062:VSN983062 WBV983062:WCJ983062 WLR983062:WMF983062 WVN983062:WWB983062">

</xml_diff>